<commit_message>
fixed organs output and added a comparison between sim versions
</commit_message>
<xml_diff>
--- a/data/CONFRONTO_VERSIONI.xlsx
+++ b/data/CONFRONTO_VERSIONI.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oem\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uniroma2-my.sharepoint.com/personal/livia_simoncini_alumni_uniroma2_eu/Documents/Corsi/Attivi/PMCSN/Progetto/PMCSN_Project/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79D3C2E9-C11C-408C-9918-E7BCF1F966EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="66" documentId="13_ncr:1_{79D3C2E9-C11C-408C-9918-E7BCF1F966EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9BF56508-CED5-48CA-A94D-566186C18DD0}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{58870B00-CDA7-45B2-A026-0B544E698EBB}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{58870B00-CDA7-45B2-A026-0B544E698EBB}"/>
   </bookViews>
   <sheets>
     <sheet name="REAL" sheetId="11" r:id="rId1"/>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1032" uniqueCount="431">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1152" uniqueCount="548">
   <si>
     <t>AB</t>
   </si>
@@ -878,138 +878,12 @@
     <t>6684.944162,+/-799.456380</t>
   </si>
   <si>
-    <t>17.906765,+/-0.476109</t>
-  </si>
-  <si>
-    <t>0.027393,+/-0.000640</t>
-  </si>
-  <si>
-    <t>33.507119,+/-0.927547</t>
-  </si>
-  <si>
-    <t>0.041680,+/-0.000953</t>
-  </si>
-  <si>
-    <t>67.539934,+/-2.881525</t>
-  </si>
-  <si>
-    <t>0.088792,+/-0.002041</t>
-  </si>
-  <si>
-    <t>144.761823,+/-6.291177</t>
-  </si>
-  <si>
-    <t>0.349264,+/-0.007850</t>
-  </si>
-  <si>
-    <t>0.050026,+/-0.000055</t>
-  </si>
-  <si>
-    <t>1002.059066,+/-66.437966</t>
-  </si>
-  <si>
-    <t>0.072007,+/-0.000097</t>
-  </si>
-  <si>
-    <t>959.409761,+/-63.425014</t>
-  </si>
-  <si>
-    <t>0.161097,+/-0.000310</t>
-  </si>
-  <si>
-    <t>997.192318,+/-66.653736</t>
-  </si>
-  <si>
-    <t>0.574853,+/-0.001421</t>
-  </si>
-  <si>
-    <t>918.586758,+/-60.895430</t>
-  </si>
-  <si>
     <t>0.000068,+/-0.000002</t>
   </si>
   <si>
-    <t>1002.009108,+/-66.437941</t>
-  </si>
-  <si>
-    <t>0.000059,+/-0.000002</t>
-  </si>
-  <si>
-    <t>959.337812,+/-63.425051</t>
-  </si>
-  <si>
-    <t>0.000057,+/-0.000002</t>
-  </si>
-  <si>
-    <t>997.031278,+/-66.653570</t>
-  </si>
-  <si>
-    <t>0.000099,+/-0.000005</t>
-  </si>
-  <si>
-    <t>918.012005,+/-60.896146</t>
-  </si>
-  <si>
-    <t>0.049958,+/-0.000056</t>
-  </si>
-  <si>
-    <t>0.071949,+/-0.000097</t>
-  </si>
-  <si>
-    <t>0.161040,+/-0.000309</t>
-  </si>
-  <si>
-    <t>0.574754,+/-0.001420</t>
-  </si>
-  <si>
-    <t>1.001364,+/-0.000031</t>
-  </si>
-  <si>
-    <t>20023.183067,+/-1322.942792</t>
-  </si>
-  <si>
-    <t>1.000818,+/-0.000034</t>
-  </si>
-  <si>
-    <t>13359.706613,+/-883.608585</t>
-  </si>
-  <si>
-    <t>1.000356,+/-0.000012</t>
-  </si>
-  <si>
-    <t>6169.723244,+/-411.995580</t>
-  </si>
-  <si>
-    <t>1.000177,+/-0.000008</t>
-  </si>
-  <si>
-    <t>1605.615741,+/-107.695190</t>
-  </si>
-  <si>
-    <t>0.001359,+/-0.000032</t>
-  </si>
-  <si>
-    <t>20022.183062,+/-1322.942792</t>
-  </si>
-  <si>
-    <t>0.000813,+/-0.000034</t>
-  </si>
-  <si>
-    <t>13358.706608,+/-883.608586</t>
-  </si>
-  <si>
     <t>0.000352,+/-0.000013</t>
   </si>
   <si>
-    <t>6168.723239,+/-411.995580</t>
-  </si>
-  <si>
-    <t>0.000172,+/-0.000008</t>
-  </si>
-  <si>
-    <t>1604.615737,+/-107.695191</t>
-  </si>
-  <si>
     <t>0.009410,+/-0.000000</t>
   </si>
   <si>
@@ -1356,6 +1230,483 @@
   </si>
   <si>
     <t>172.920673,+/-25.154627</t>
+  </si>
+  <si>
+    <t>18.820131,+/-0.167493</t>
+  </si>
+  <si>
+    <t>0.023754,+/-0.000005</t>
+  </si>
+  <si>
+    <t>33.858655,+/-0.317220</t>
+  </si>
+  <si>
+    <t>0.036955,+/-0.000029</t>
+  </si>
+  <si>
+    <t>39.351068,+/-1.189536</t>
+  </si>
+  <si>
+    <t>0.077140,+/-0.000043</t>
+  </si>
+  <si>
+    <t>118.897982,+/-3.170431</t>
+  </si>
+  <si>
+    <t>0.313077,+/-0.000267</t>
+  </si>
+  <si>
+    <t>0.040567,+/-0.000633</t>
+  </si>
+  <si>
+    <t>357.592161,+/-22.601821</t>
+  </si>
+  <si>
+    <t>0.062997,+/-0.000778</t>
+  </si>
+  <si>
+    <t>460.076237,+/-29.650828</t>
+  </si>
+  <si>
+    <t>0.195510,+/-0.000234</t>
+  </si>
+  <si>
+    <t>1333.428791,+/-87.368928</t>
+  </si>
+  <si>
+    <t>0.730260,+/-0.001532</t>
+  </si>
+  <si>
+    <t>1305.637873,+/-85.652780</t>
+  </si>
+  <si>
+    <t>0.000069,+/-0.000001</t>
+  </si>
+  <si>
+    <t>357.551663,+/-22.601523</t>
+  </si>
+  <si>
+    <t>0.000103,+/-0.000002</t>
+  </si>
+  <si>
+    <t>460.013343,+/-29.650498</t>
+  </si>
+  <si>
+    <t>0.000838,+/-0.000027</t>
+  </si>
+  <si>
+    <t>1333.234118,+/-87.368971</t>
+  </si>
+  <si>
+    <t>0.005864,+/-0.000316</t>
+  </si>
+  <si>
+    <t>1304.913477,+/-85.652453</t>
+  </si>
+  <si>
+    <t>0.040498,+/-0.000633</t>
+  </si>
+  <si>
+    <t>0.062894,+/-0.000780</t>
+  </si>
+  <si>
+    <t>0.194672,+/-0.000241</t>
+  </si>
+  <si>
+    <t>0.724396,+/-0.001441</t>
+  </si>
+  <si>
+    <t>1.001733,+/-0.000042</t>
+  </si>
+  <si>
+    <t>8732.718413,+/-535.749395</t>
+  </si>
+  <si>
+    <t>1.001661,+/-0.000047</t>
+  </si>
+  <si>
+    <t>7248.399349,+/-456.651434</t>
+  </si>
+  <si>
+    <t>1.004310,+/-0.000137</t>
+  </si>
+  <si>
+    <t>6855.296325,+/-449.336210</t>
+  </si>
+  <si>
+    <t>1.008091,+/-0.000436</t>
+  </si>
+  <si>
+    <t>1799.650588,+/-118.074264</t>
+  </si>
+  <si>
+    <t>0.001728,+/-0.000042</t>
+  </si>
+  <si>
+    <t>8731.718409,+/-535.749396</t>
+  </si>
+  <si>
+    <t>0.001657,+/-0.000046</t>
+  </si>
+  <si>
+    <t>7247.399344,+/-456.651435</t>
+  </si>
+  <si>
+    <t>0.004305,+/-0.000138</t>
+  </si>
+  <si>
+    <t>6854.296321,+/-449.336210</t>
+  </si>
+  <si>
+    <t>0.008087,+/-0.000436</t>
+  </si>
+  <si>
+    <t>1798.650583,+/-118.074265</t>
+  </si>
+  <si>
+    <t>0.068797,+/-0.000030</t>
+  </si>
+  <si>
+    <t>0.087495,+/-0.000070</t>
+  </si>
+  <si>
+    <t>0.278202,+/-0.000308</t>
+  </si>
+  <si>
+    <t>0.937549,+/-0.002864</t>
+  </si>
+  <si>
+    <t>433.743576,+/-126.904959</t>
+  </si>
+  <si>
+    <t>212.057910,+/-67.927223</t>
+  </si>
+  <si>
+    <t>0.372527,+/-0.291970</t>
+  </si>
+  <si>
+    <t>18.338724,+/-0.430583</t>
+  </si>
+  <si>
+    <t>0.027542,+/-0.000585</t>
+  </si>
+  <si>
+    <t>32.554669,+/-0.917668</t>
+  </si>
+  <si>
+    <t>0.041811,+/-0.000875</t>
+  </si>
+  <si>
+    <t>69.055962,+/-3.030271</t>
+  </si>
+  <si>
+    <t>0.089074,+/-0.001865</t>
+  </si>
+  <si>
+    <t>130.898519,+/-5.940377</t>
+  </si>
+  <si>
+    <t>0.342317,+/-0.007923</t>
+  </si>
+  <si>
+    <t>0.051829,+/-0.000041</t>
+  </si>
+  <si>
+    <t>955.851363,+/-67.472107</t>
+  </si>
+  <si>
+    <t>0.073246,+/-0.000092</t>
+  </si>
+  <si>
+    <t>893.506992,+/-63.094818</t>
+  </si>
+  <si>
+    <t>0.164545,+/-0.000383</t>
+  </si>
+  <si>
+    <t>942.257255,+/-66.742252</t>
+  </si>
+  <si>
+    <t>0.382874,+/-0.008703</t>
+  </si>
+  <si>
+    <t>22.557051,+/-1.266756</t>
+  </si>
+  <si>
+    <t>0.000259,+/-0.000006</t>
+  </si>
+  <si>
+    <t>955.799793,+/-67.472122</t>
+  </si>
+  <si>
+    <t>0.000100,+/-0.000003</t>
+  </si>
+  <si>
+    <t>893.433846,+/-63.094865</t>
+  </si>
+  <si>
+    <t>0.000087,+/-0.000004</t>
+  </si>
+  <si>
+    <t>942.092797,+/-66.742184</t>
+  </si>
+  <si>
+    <t>0.000078,+/-0.000004</t>
+  </si>
+  <si>
+    <t>22.174254,+/-1.261777</t>
+  </si>
+  <si>
+    <t>0.051570,+/-0.000037</t>
+  </si>
+  <si>
+    <t>0.073146,+/-0.000090</t>
+  </si>
+  <si>
+    <t>0.164458,+/-0.000380</t>
+  </si>
+  <si>
+    <t>0.382796,+/-0.008705</t>
+  </si>
+  <si>
+    <t>1.005021,+/-0.000109</t>
+  </si>
+  <si>
+    <t>18554.696408,+/-1313.445550</t>
+  </si>
+  <si>
+    <t>1.001372,+/-0.000038</t>
+  </si>
+  <si>
+    <t>12243.467313,+/-869.192398</t>
+  </si>
+  <si>
+    <t>1.000534,+/-0.000021</t>
+  </si>
+  <si>
+    <t>5721.831648,+/-407.963731</t>
+  </si>
+  <si>
+    <t>1.000218,+/-0.000012</t>
+  </si>
+  <si>
+    <t>58.253493,+/-2.899239</t>
+  </si>
+  <si>
+    <t>0.005017,+/-0.000108</t>
+  </si>
+  <si>
+    <t>18553.696404,+/-1313.445550</t>
+  </si>
+  <si>
+    <t>0.001368,+/-0.000038</t>
+  </si>
+  <si>
+    <t>12242.467309,+/-869.192399</t>
+  </si>
+  <si>
+    <t>0.000530,+/-0.000021</t>
+  </si>
+  <si>
+    <t>5720.831643,+/-407.963732</t>
+  </si>
+  <si>
+    <t>0.000214,+/-0.000013</t>
+  </si>
+  <si>
+    <t>57.253489,+/-2.899240</t>
+  </si>
+  <si>
+    <t>0.010140,+/-0.000000</t>
+  </si>
+  <si>
+    <t>0.082811,+/-0.000044</t>
+  </si>
+  <si>
+    <t>0.105204,+/-0.000099</t>
+  </si>
+  <si>
+    <t>0.334888,+/-0.000338</t>
+  </si>
+  <si>
+    <t>1.147017,+/-0.003754</t>
+  </si>
+  <si>
+    <t>0.016165,+/-0.027087</t>
+  </si>
+  <si>
+    <t>0.020552,+/-0.032145</t>
+  </si>
+  <si>
+    <t>0.004047,+/-0.006428</t>
+  </si>
+  <si>
+    <t>0.599098,+/-0.134936</t>
+  </si>
+  <si>
+    <t>746.366385,+/-2.914710</t>
+  </si>
+  <si>
+    <t>43.159385,+/-1.456315</t>
+  </si>
+  <si>
+    <t>17.866809,+/-0.472035</t>
+  </si>
+  <si>
+    <t>0.027362,+/-0.000631</t>
+  </si>
+  <si>
+    <t>33.427146,+/-0.918869</t>
+  </si>
+  <si>
+    <t>0.041629,+/-0.000942</t>
+  </si>
+  <si>
+    <t>67.458916,+/-2.891160</t>
+  </si>
+  <si>
+    <t>0.088446,+/-0.002021</t>
+  </si>
+  <si>
+    <t>144.333410,+/-6.265642</t>
+  </si>
+  <si>
+    <t>0.350511,+/-0.007974</t>
+  </si>
+  <si>
+    <t>0.050136,+/-0.000057</t>
+  </si>
+  <si>
+    <t>1001.654117,+/-66.921810</t>
+  </si>
+  <si>
+    <t>0.072034,+/-0.000111</t>
+  </si>
+  <si>
+    <t>957.251136,+/-63.653846</t>
+  </si>
+  <si>
+    <t>0.159967,+/-0.000379</t>
+  </si>
+  <si>
+    <t>993.553887,+/-66.788939</t>
+  </si>
+  <si>
+    <t>0.570764,+/-0.001633</t>
+  </si>
+  <si>
+    <t>905.799234,+/-61.046612</t>
+  </si>
+  <si>
+    <t>1001.604050,+/-66.921791</t>
+  </si>
+  <si>
+    <t>0.000059,+/-0.000003</t>
+  </si>
+  <si>
+    <t>957.179160,+/-63.653910</t>
+  </si>
+  <si>
+    <t>0.000056,+/-0.000002</t>
+  </si>
+  <si>
+    <t>993.393976,+/-66.788720</t>
+  </si>
+  <si>
+    <t>0.000098,+/-0.000005</t>
+  </si>
+  <si>
+    <t>905.228568,+/-61.045979</t>
+  </si>
+  <si>
+    <t>0.050068,+/-0.000058</t>
+  </si>
+  <si>
+    <t>0.071976,+/-0.000109</t>
+  </si>
+  <si>
+    <t>0.159911,+/-0.000377</t>
+  </si>
+  <si>
+    <t>0.570666,+/-0.001633</t>
+  </si>
+  <si>
+    <t>1.001366,+/-0.000031</t>
+  </si>
+  <si>
+    <t>19979.769017,+/-1331.300842</t>
+  </si>
+  <si>
+    <t>1.000820,+/-0.000034</t>
+  </si>
+  <si>
+    <t>13341.840366,+/-889.006732</t>
+  </si>
+  <si>
+    <t>1.000357,+/-0.000012</t>
+  </si>
+  <si>
+    <t>6183.145236,+/-415.002467</t>
+  </si>
+  <si>
+    <t>1.000178,+/-0.000008</t>
+  </si>
+  <si>
+    <t>1581.140947,+/-106.062699</t>
+  </si>
+  <si>
+    <t>0.001361,+/-0.000031</t>
+  </si>
+  <si>
+    <t>19978.769012,+/-1331.300843</t>
+  </si>
+  <si>
+    <t>0.000815,+/-0.000034</t>
+  </si>
+  <si>
+    <t>13340.840361,+/-889.006733</t>
+  </si>
+  <si>
+    <t>6182.145231,+/-415.002468</t>
+  </si>
+  <si>
+    <t>0.000173,+/-0.000008</t>
+  </si>
+  <si>
+    <t>1580.140941,+/-106.062700</t>
+  </si>
+  <si>
+    <t>0.009455,+/-0.000000</t>
+  </si>
+  <si>
+    <t>0.082822,+/-0.000042</t>
+  </si>
+  <si>
+    <t>0.105211,+/-0.000093</t>
+  </si>
+  <si>
+    <t>0.334907,+/-0.000316</t>
+  </si>
+  <si>
+    <t>1.147517,+/-0.003508</t>
+  </si>
+  <si>
+    <t>0.295573,+/-0.302875</t>
+  </si>
+  <si>
+    <t>0.379164,+/-0.363008</t>
+  </si>
+  <si>
+    <t>0.084400,+/-0.083133</t>
+  </si>
+  <si>
+    <t>0.001251,+/-0.001002</t>
+  </si>
+  <si>
+    <t>2126.627884,+/-19.297079</t>
+  </si>
+  <si>
+    <t>42.779000,+/-1.372047</t>
   </si>
 </sst>
 </file>
@@ -2519,8 +2870,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7EFBA70C-A8ED-4C94-8FF2-9C7F6AB93B1B}">
   <dimension ref="A1:G145"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
-      <selection activeCell="D113" sqref="D113"/>
+    <sheetView topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="D82" sqref="D82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2575,7 +2926,7 @@
         <v>164</v>
       </c>
       <c r="F3">
-        <v>241</v>
+        <v>193</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
@@ -2589,7 +2940,7 @@
         <v>119260</v>
       </c>
       <c r="F4">
-        <v>160593</v>
+        <v>153587</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -2606,7 +2957,7 @@
         <v>121</v>
       </c>
       <c r="F5">
-        <v>126</v>
+        <v>106</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
@@ -2620,7 +2971,7 @@
         <v>84724</v>
       </c>
       <c r="F6">
-        <v>106205</v>
+        <v>98882</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
@@ -2637,7 +2988,7 @@
         <v>52</v>
       </c>
       <c r="F7">
-        <v>75</v>
+        <v>96</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
@@ -2651,7 +3002,7 @@
         <v>36100</v>
       </c>
       <c r="F8">
-        <v>49755</v>
+        <v>47340</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
@@ -2668,7 +3019,7 @@
         <v>16</v>
       </c>
       <c r="F9">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
@@ -2682,7 +3033,7 @@
         <v>10730</v>
       </c>
       <c r="F10">
-        <v>12767</v>
+        <v>11638</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
@@ -2716,7 +3067,7 @@
         <v>12481</v>
       </c>
       <c r="F12">
-        <v>15195</v>
+        <v>10620</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
@@ -2747,7 +3098,7 @@
         <v>7932</v>
       </c>
       <c r="F14">
-        <v>7463</v>
+        <v>4665</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
@@ -2778,7 +3129,7 @@
         <v>5497</v>
       </c>
       <c r="F16">
-        <v>4707</v>
+        <v>4436</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
@@ -2809,7 +3160,7 @@
         <v>1469</v>
       </c>
       <c r="F18">
-        <v>641</v>
+        <v>588</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
@@ -2843,7 +3194,7 @@
         <v>15988</v>
       </c>
       <c r="F20">
-        <v>25308</v>
+        <v>27392</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
@@ -2874,7 +3225,7 @@
         <v>10725</v>
       </c>
       <c r="F22">
-        <v>13985</v>
+        <v>16852</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
@@ -2905,7 +3256,7 @@
         <v>6347</v>
       </c>
       <c r="F24">
-        <v>7604</v>
+        <v>12034</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
@@ -2936,7 +3287,7 @@
         <v>1755</v>
       </c>
       <c r="F26">
-        <v>1320</v>
+        <v>2519</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
@@ -2950,13 +3301,13 @@
         <v>8</v>
       </c>
       <c r="D27" t="s">
-        <v>375</v>
+        <v>333</v>
       </c>
       <c r="E27" t="s">
-        <v>319</v>
+        <v>277</v>
       </c>
       <c r="F27" t="s">
-        <v>271</v>
+        <v>389</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
@@ -2964,13 +3315,13 @@
         <v>7</v>
       </c>
       <c r="D28" t="s">
-        <v>376</v>
+        <v>334</v>
       </c>
       <c r="E28" t="s">
-        <v>320</v>
+        <v>278</v>
       </c>
       <c r="F28" t="s">
-        <v>272</v>
+        <v>390</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
@@ -2981,13 +3332,13 @@
         <v>8</v>
       </c>
       <c r="D29" t="s">
-        <v>377</v>
+        <v>335</v>
       </c>
       <c r="E29" t="s">
-        <v>321</v>
+        <v>279</v>
       </c>
       <c r="F29" t="s">
-        <v>273</v>
+        <v>391</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
@@ -2995,13 +3346,13 @@
         <v>7</v>
       </c>
       <c r="D30" t="s">
-        <v>378</v>
+        <v>336</v>
       </c>
       <c r="E30" t="s">
-        <v>322</v>
+        <v>280</v>
       </c>
       <c r="F30" t="s">
-        <v>274</v>
+        <v>392</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
@@ -3012,13 +3363,13 @@
         <v>8</v>
       </c>
       <c r="D31" t="s">
-        <v>379</v>
+        <v>337</v>
       </c>
       <c r="E31" t="s">
-        <v>323</v>
+        <v>281</v>
       </c>
       <c r="F31" t="s">
-        <v>275</v>
+        <v>393</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
@@ -3026,13 +3377,13 @@
         <v>7</v>
       </c>
       <c r="D32" t="s">
-        <v>380</v>
+        <v>338</v>
       </c>
       <c r="E32" t="s">
-        <v>324</v>
+        <v>282</v>
       </c>
       <c r="F32" t="s">
-        <v>276</v>
+        <v>394</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
@@ -3043,13 +3394,13 @@
         <v>8</v>
       </c>
       <c r="D33" t="s">
-        <v>381</v>
+        <v>339</v>
       </c>
       <c r="E33" t="s">
-        <v>325</v>
+        <v>283</v>
       </c>
       <c r="F33" t="s">
-        <v>277</v>
+        <v>395</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
@@ -3057,13 +3408,13 @@
         <v>7</v>
       </c>
       <c r="D34" t="s">
-        <v>382</v>
+        <v>340</v>
       </c>
       <c r="E34" t="s">
-        <v>326</v>
+        <v>284</v>
       </c>
       <c r="F34" t="s">
-        <v>278</v>
+        <v>396</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
@@ -3077,13 +3428,13 @@
         <v>8</v>
       </c>
       <c r="D35" t="s">
-        <v>383</v>
+        <v>341</v>
       </c>
       <c r="E35" t="s">
-        <v>327</v>
+        <v>285</v>
       </c>
       <c r="F35" t="s">
-        <v>279</v>
+        <v>397</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
@@ -3091,13 +3442,13 @@
         <v>7</v>
       </c>
       <c r="D36" t="s">
-        <v>384</v>
+        <v>342</v>
       </c>
       <c r="E36" t="s">
-        <v>328</v>
+        <v>286</v>
       </c>
       <c r="F36" t="s">
-        <v>280</v>
+        <v>398</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
@@ -3108,13 +3459,13 @@
         <v>8</v>
       </c>
       <c r="D37" t="s">
-        <v>385</v>
+        <v>343</v>
       </c>
       <c r="E37" t="s">
-        <v>329</v>
+        <v>287</v>
       </c>
       <c r="F37" t="s">
-        <v>281</v>
+        <v>399</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
@@ -3122,13 +3473,13 @@
         <v>7</v>
       </c>
       <c r="D38" t="s">
-        <v>386</v>
+        <v>344</v>
       </c>
       <c r="E38" t="s">
-        <v>330</v>
+        <v>288</v>
       </c>
       <c r="F38" t="s">
-        <v>282</v>
+        <v>400</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
@@ -3139,13 +3490,13 @@
         <v>8</v>
       </c>
       <c r="D39" t="s">
-        <v>387</v>
+        <v>345</v>
       </c>
       <c r="E39" t="s">
-        <v>331</v>
+        <v>289</v>
       </c>
       <c r="F39" t="s">
-        <v>283</v>
+        <v>401</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
@@ -3153,13 +3504,13 @@
         <v>7</v>
       </c>
       <c r="D40" t="s">
-        <v>388</v>
+        <v>346</v>
       </c>
       <c r="E40" t="s">
-        <v>332</v>
+        <v>290</v>
       </c>
       <c r="F40" t="s">
-        <v>284</v>
+        <v>402</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
@@ -3170,13 +3521,13 @@
         <v>8</v>
       </c>
       <c r="D41" t="s">
-        <v>389</v>
+        <v>347</v>
       </c>
       <c r="E41" t="s">
-        <v>333</v>
+        <v>291</v>
       </c>
       <c r="F41" t="s">
-        <v>285</v>
+        <v>403</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
@@ -3184,13 +3535,13 @@
         <v>7</v>
       </c>
       <c r="D42" t="s">
-        <v>390</v>
+        <v>348</v>
       </c>
       <c r="E42" t="s">
-        <v>334</v>
+        <v>292</v>
       </c>
       <c r="F42" t="s">
-        <v>286</v>
+        <v>404</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
@@ -3204,13 +3555,13 @@
         <v>8</v>
       </c>
       <c r="D43" t="s">
-        <v>391</v>
+        <v>349</v>
       </c>
       <c r="E43" t="s">
-        <v>335</v>
+        <v>293</v>
       </c>
       <c r="F43" t="s">
-        <v>287</v>
+        <v>405</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
@@ -3218,13 +3569,13 @@
         <v>7</v>
       </c>
       <c r="D44" t="s">
-        <v>392</v>
+        <v>350</v>
       </c>
       <c r="E44" t="s">
-        <v>336</v>
+        <v>294</v>
       </c>
       <c r="F44" t="s">
-        <v>288</v>
+        <v>406</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.2">
@@ -3235,13 +3586,13 @@
         <v>8</v>
       </c>
       <c r="D45" t="s">
-        <v>393</v>
+        <v>351</v>
       </c>
       <c r="E45" t="s">
-        <v>337</v>
+        <v>295</v>
       </c>
       <c r="F45" t="s">
-        <v>289</v>
+        <v>407</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.2">
@@ -3249,13 +3600,13 @@
         <v>7</v>
       </c>
       <c r="D46" t="s">
-        <v>394</v>
+        <v>352</v>
       </c>
       <c r="E46" t="s">
-        <v>338</v>
+        <v>296</v>
       </c>
       <c r="F46" t="s">
-        <v>290</v>
+        <v>408</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.2">
@@ -3266,13 +3617,13 @@
         <v>8</v>
       </c>
       <c r="D47" t="s">
-        <v>395</v>
+        <v>353</v>
       </c>
       <c r="E47" t="s">
-        <v>339</v>
+        <v>297</v>
       </c>
       <c r="F47" t="s">
-        <v>291</v>
+        <v>409</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.2">
@@ -3280,13 +3631,13 @@
         <v>7</v>
       </c>
       <c r="D48" t="s">
-        <v>396</v>
+        <v>354</v>
       </c>
       <c r="E48" t="s">
-        <v>340</v>
+        <v>298</v>
       </c>
       <c r="F48" t="s">
-        <v>292</v>
+        <v>410</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.2">
@@ -3297,13 +3648,13 @@
         <v>8</v>
       </c>
       <c r="D49" t="s">
-        <v>397</v>
+        <v>355</v>
       </c>
       <c r="E49" t="s">
-        <v>341</v>
+        <v>299</v>
       </c>
       <c r="F49" t="s">
-        <v>293</v>
+        <v>411</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.2">
@@ -3311,13 +3662,13 @@
         <v>7</v>
       </c>
       <c r="D50" t="s">
-        <v>398</v>
+        <v>356</v>
       </c>
       <c r="E50" t="s">
-        <v>342</v>
+        <v>300</v>
       </c>
       <c r="F50" t="s">
-        <v>294</v>
+        <v>412</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.2">
@@ -3328,13 +3679,13 @@
         <v>3</v>
       </c>
       <c r="D51" t="s">
-        <v>399</v>
+        <v>357</v>
       </c>
       <c r="E51" t="s">
-        <v>343</v>
+        <v>301</v>
       </c>
       <c r="F51" t="s">
-        <v>295</v>
+        <v>413</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.2">
@@ -3342,13 +3693,13 @@
         <v>2</v>
       </c>
       <c r="D52" t="s">
-        <v>400</v>
+        <v>358</v>
       </c>
       <c r="E52" t="s">
-        <v>344</v>
+        <v>302</v>
       </c>
       <c r="F52" t="s">
-        <v>296</v>
+        <v>414</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.2">
@@ -3356,13 +3707,13 @@
         <v>1</v>
       </c>
       <c r="D53" t="s">
-        <v>401</v>
+        <v>359</v>
       </c>
       <c r="E53" t="s">
-        <v>345</v>
+        <v>303</v>
       </c>
       <c r="F53" t="s">
-        <v>297</v>
+        <v>415</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.2">
@@ -3370,13 +3721,13 @@
         <v>0</v>
       </c>
       <c r="D54" t="s">
-        <v>402</v>
+        <v>360</v>
       </c>
       <c r="E54" t="s">
-        <v>346</v>
+        <v>304</v>
       </c>
       <c r="F54" t="s">
-        <v>298</v>
+        <v>416</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.2">
@@ -3390,13 +3741,13 @@
         <v>8</v>
       </c>
       <c r="D55" t="s">
-        <v>403</v>
+        <v>361</v>
       </c>
       <c r="E55" t="s">
-        <v>347</v>
+        <v>305</v>
       </c>
       <c r="F55" t="s">
-        <v>299</v>
+        <v>417</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.2">
@@ -3404,13 +3755,13 @@
         <v>7</v>
       </c>
       <c r="D56" t="s">
-        <v>404</v>
+        <v>362</v>
       </c>
       <c r="E56" t="s">
-        <v>348</v>
+        <v>306</v>
       </c>
       <c r="F56" t="s">
-        <v>300</v>
+        <v>418</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.2">
@@ -3421,13 +3772,13 @@
         <v>8</v>
       </c>
       <c r="D57" t="s">
-        <v>405</v>
+        <v>363</v>
       </c>
       <c r="E57" t="s">
-        <v>349</v>
+        <v>307</v>
       </c>
       <c r="F57" t="s">
-        <v>301</v>
+        <v>419</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.2">
@@ -3435,13 +3786,13 @@
         <v>7</v>
       </c>
       <c r="D58" t="s">
-        <v>406</v>
+        <v>364</v>
       </c>
       <c r="E58" t="s">
-        <v>350</v>
+        <v>308</v>
       </c>
       <c r="F58" t="s">
-        <v>302</v>
+        <v>420</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.2">
@@ -3452,13 +3803,13 @@
         <v>8</v>
       </c>
       <c r="D59" t="s">
-        <v>407</v>
+        <v>365</v>
       </c>
       <c r="E59" t="s">
-        <v>351</v>
+        <v>309</v>
       </c>
       <c r="F59" t="s">
-        <v>303</v>
+        <v>421</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.2">
@@ -3466,13 +3817,13 @@
         <v>7</v>
       </c>
       <c r="D60" t="s">
-        <v>408</v>
+        <v>366</v>
       </c>
       <c r="E60" t="s">
-        <v>352</v>
+        <v>310</v>
       </c>
       <c r="F60" t="s">
-        <v>304</v>
+        <v>422</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.2">
@@ -3483,13 +3834,13 @@
         <v>8</v>
       </c>
       <c r="D61" t="s">
-        <v>409</v>
+        <v>367</v>
       </c>
       <c r="E61" t="s">
-        <v>353</v>
+        <v>311</v>
       </c>
       <c r="F61" t="s">
-        <v>305</v>
+        <v>423</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.2">
@@ -3497,13 +3848,13 @@
         <v>7</v>
       </c>
       <c r="D62" t="s">
-        <v>410</v>
+        <v>368</v>
       </c>
       <c r="E62" t="s">
-        <v>354</v>
+        <v>312</v>
       </c>
       <c r="F62" t="s">
-        <v>306</v>
+        <v>424</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.2">
@@ -3517,13 +3868,13 @@
         <v>8</v>
       </c>
       <c r="D63" t="s">
-        <v>411</v>
+        <v>369</v>
       </c>
       <c r="E63" t="s">
-        <v>355</v>
+        <v>313</v>
       </c>
       <c r="F63" t="s">
-        <v>307</v>
+        <v>425</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.2">
@@ -3531,13 +3882,13 @@
         <v>7</v>
       </c>
       <c r="D64" t="s">
-        <v>412</v>
+        <v>370</v>
       </c>
       <c r="E64" t="s">
-        <v>356</v>
+        <v>314</v>
       </c>
       <c r="F64" t="s">
-        <v>308</v>
+        <v>426</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.2">
@@ -3548,13 +3899,13 @@
         <v>8</v>
       </c>
       <c r="D65" t="s">
-        <v>413</v>
+        <v>371</v>
       </c>
       <c r="E65" t="s">
-        <v>357</v>
+        <v>315</v>
       </c>
       <c r="F65" t="s">
-        <v>309</v>
+        <v>427</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.2">
@@ -3562,13 +3913,13 @@
         <v>7</v>
       </c>
       <c r="D66" t="s">
-        <v>414</v>
+        <v>372</v>
       </c>
       <c r="E66" t="s">
-        <v>358</v>
+        <v>316</v>
       </c>
       <c r="F66" t="s">
-        <v>310</v>
+        <v>428</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.2">
@@ -3579,13 +3930,13 @@
         <v>8</v>
       </c>
       <c r="D67" t="s">
-        <v>415</v>
+        <v>373</v>
       </c>
       <c r="E67" t="s">
-        <v>359</v>
+        <v>317</v>
       </c>
       <c r="F67" t="s">
-        <v>311</v>
+        <v>429</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.2">
@@ -3593,13 +3944,13 @@
         <v>7</v>
       </c>
       <c r="D68" t="s">
-        <v>416</v>
+        <v>374</v>
       </c>
       <c r="E68" t="s">
-        <v>360</v>
+        <v>318</v>
       </c>
       <c r="F68" t="s">
-        <v>312</v>
+        <v>430</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.2">
@@ -3610,13 +3961,13 @@
         <v>8</v>
       </c>
       <c r="D69" t="s">
-        <v>417</v>
+        <v>375</v>
       </c>
       <c r="E69" t="s">
-        <v>361</v>
+        <v>319</v>
       </c>
       <c r="F69" t="s">
-        <v>313</v>
+        <v>431</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.2">
@@ -3624,13 +3975,13 @@
         <v>7</v>
       </c>
       <c r="D70" t="s">
-        <v>418</v>
+        <v>376</v>
       </c>
       <c r="E70" t="s">
-        <v>362</v>
+        <v>320</v>
       </c>
       <c r="F70" t="s">
-        <v>314</v>
+        <v>432</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.2">
@@ -3638,13 +3989,13 @@
         <v>41</v>
       </c>
       <c r="D71" t="s">
-        <v>419</v>
+        <v>377</v>
       </c>
       <c r="E71" t="s">
-        <v>363</v>
+        <v>321</v>
       </c>
       <c r="F71" t="s">
-        <v>315</v>
+        <v>273</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.2">
@@ -3683,6 +4034,9 @@
       <c r="E74">
         <v>82091</v>
       </c>
+      <c r="F74">
+        <v>91943</v>
+      </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B75" t="s">
@@ -3694,6 +4048,9 @@
       <c r="E75">
         <v>63585</v>
       </c>
+      <c r="F75">
+        <v>72086</v>
+      </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B76" t="s">
@@ -3705,6 +4062,9 @@
       <c r="E76">
         <v>21438</v>
       </c>
+      <c r="F76">
+        <v>22775</v>
+      </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B77" t="s">
@@ -3715,6 +4075,9 @@
       </c>
       <c r="E77">
         <v>6088</v>
+      </c>
+      <c r="F77">
+        <v>6650</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.2">
@@ -3730,6 +4093,9 @@
       <c r="E78">
         <v>95235</v>
       </c>
+      <c r="F78">
+        <v>74596</v>
+      </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B79" t="s">
@@ -3741,6 +4107,9 @@
       <c r="E79">
         <v>40273</v>
       </c>
+      <c r="F79">
+        <v>32697</v>
+      </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B80" t="s">
@@ -3752,6 +4121,9 @@
       <c r="E80">
         <v>13201</v>
       </c>
+      <c r="F80">
+        <v>9830</v>
+      </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B81" t="s">
@@ -3762,6 +4134,9 @@
       </c>
       <c r="E81">
         <v>1459</v>
+      </c>
+      <c r="F81">
+        <v>1947</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.2">
@@ -3777,6 +4152,9 @@
       <c r="E82">
         <v>4227</v>
       </c>
+      <c r="F82">
+        <v>1869</v>
+      </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B83" t="s">
@@ -3788,6 +4166,9 @@
       <c r="E83">
         <v>3154</v>
       </c>
+      <c r="F83">
+        <v>1650</v>
+      </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B84" t="s">
@@ -3799,6 +4180,9 @@
       <c r="E84">
         <v>2505</v>
       </c>
+      <c r="F84">
+        <v>335</v>
+      </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B85" t="s">
@@ -3809,6 +4193,9 @@
       </c>
       <c r="E85">
         <v>6</v>
+      </c>
+      <c r="F85">
+        <v>23</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.2">
@@ -3819,10 +4206,13 @@
         <v>3</v>
       </c>
       <c r="D86" t="s">
-        <v>420</v>
+        <v>378</v>
       </c>
       <c r="E86" t="s">
-        <v>364</v>
+        <v>322</v>
+      </c>
+      <c r="F86" t="s">
+        <v>433</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.2">
@@ -3830,10 +4220,13 @@
         <v>2</v>
       </c>
       <c r="D87" t="s">
-        <v>421</v>
+        <v>379</v>
       </c>
       <c r="E87" t="s">
-        <v>365</v>
+        <v>323</v>
+      </c>
+      <c r="F87" t="s">
+        <v>434</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.2">
@@ -3841,10 +4234,13 @@
         <v>1</v>
       </c>
       <c r="D88" t="s">
-        <v>422</v>
+        <v>380</v>
       </c>
       <c r="E88" t="s">
-        <v>366</v>
+        <v>324</v>
+      </c>
+      <c r="F88" t="s">
+        <v>435</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.2">
@@ -3852,10 +4248,13 @@
         <v>0</v>
       </c>
       <c r="D89" t="s">
-        <v>423</v>
+        <v>381</v>
       </c>
       <c r="E89" t="s">
-        <v>367</v>
+        <v>325</v>
+      </c>
+      <c r="F89" t="s">
+        <v>436</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.2">
@@ -3866,10 +4265,13 @@
         <v>3</v>
       </c>
       <c r="D90" t="s">
-        <v>424</v>
+        <v>382</v>
       </c>
       <c r="E90" t="s">
-        <v>368</v>
+        <v>326</v>
+      </c>
+      <c r="F90" t="s">
+        <v>437</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.2">
@@ -3877,10 +4279,13 @@
         <v>2</v>
       </c>
       <c r="D91" t="s">
-        <v>425</v>
+        <v>383</v>
       </c>
       <c r="E91" t="s">
-        <v>369</v>
+        <v>327</v>
+      </c>
+      <c r="F91" t="s">
+        <v>438</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.2">
@@ -3888,10 +4293,13 @@
         <v>1</v>
       </c>
       <c r="D92" t="s">
-        <v>426</v>
+        <v>384</v>
       </c>
       <c r="E92" t="s">
-        <v>370</v>
+        <v>328</v>
+      </c>
+      <c r="F92" t="s">
+        <v>439</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.2">
@@ -3899,10 +4307,13 @@
         <v>0</v>
       </c>
       <c r="D93" t="s">
-        <v>427</v>
+        <v>385</v>
       </c>
       <c r="E93" t="s">
-        <v>371</v>
+        <v>329</v>
+      </c>
+      <c r="F93" t="s">
+        <v>275</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.2">
@@ -4060,13 +4471,13 @@
         <v>20</v>
       </c>
       <c r="D104" t="s">
-        <v>428</v>
+        <v>386</v>
       </c>
       <c r="E104" t="s">
-        <v>372</v>
+        <v>330</v>
       </c>
       <c r="F104" t="s">
-        <v>316</v>
+        <v>274</v>
       </c>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.2">
@@ -4153,13 +4564,13 @@
         <v>26</v>
       </c>
       <c r="D111" t="s">
-        <v>429</v>
+        <v>387</v>
       </c>
       <c r="E111" t="s">
-        <v>373</v>
+        <v>331</v>
       </c>
       <c r="F111" t="s">
-        <v>317</v>
+        <v>275</v>
       </c>
       <c r="G111" s="9"/>
     </row>
@@ -4168,13 +4579,13 @@
         <v>25</v>
       </c>
       <c r="D112" t="s">
-        <v>430</v>
+        <v>388</v>
       </c>
       <c r="E112" t="s">
-        <v>374</v>
+        <v>332</v>
       </c>
       <c r="F112" t="s">
-        <v>318</v>
+        <v>276</v>
       </c>
       <c r="G112" s="9"/>
     </row>
@@ -4211,8 +4622,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4B0CFC0-6B65-4A53-A15E-ECBF83434F62}">
   <dimension ref="A1:F120"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G109" sqref="G109"/>
+    <sheetView topLeftCell="A69" workbookViewId="0">
+      <selection activeCell="F121" sqref="F121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4262,6 +4673,9 @@
       <c r="E3">
         <v>179</v>
       </c>
+      <c r="F3">
+        <v>227</v>
+      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C4" t="s">
@@ -4272,6 +4686,9 @@
       </c>
       <c r="E4">
         <v>131959</v>
+      </c>
+      <c r="F4">
+        <v>152041</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
@@ -4287,6 +4704,9 @@
       <c r="E5">
         <v>134</v>
       </c>
+      <c r="F5">
+        <v>121</v>
+      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C6" t="s">
@@ -4297,6 +4717,9 @@
       </c>
       <c r="E6">
         <v>94704</v>
+      </c>
+      <c r="F6">
+        <v>100509</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -4312,6 +4735,9 @@
       <c r="E7">
         <v>62</v>
       </c>
+      <c r="F7">
+        <v>65</v>
+      </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C8" t="s">
@@ -4323,6 +4749,9 @@
       <c r="E8">
         <v>39946</v>
       </c>
+      <c r="F8">
+        <v>47151</v>
+      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
@@ -4337,6 +4766,9 @@
       <c r="E9">
         <v>16</v>
       </c>
+      <c r="F9">
+        <v>28</v>
+      </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C10" t="s">
@@ -4347,6 +4779,9 @@
       </c>
       <c r="E10">
         <v>12107</v>
+      </c>
+      <c r="F10">
+        <v>11905</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
@@ -4365,6 +4800,9 @@
       <c r="E11">
         <v>1</v>
       </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C12" t="s">
@@ -4375,6 +4813,9 @@
       </c>
       <c r="E12">
         <v>16221</v>
+      </c>
+      <c r="F12">
+        <v>14571</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
@@ -4390,6 +4831,9 @@
       <c r="E13">
         <v>0</v>
       </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C14" t="s">
@@ -4400,6 +4844,9 @@
       </c>
       <c r="E14">
         <v>8211</v>
+      </c>
+      <c r="F14">
+        <v>6975</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
@@ -4415,6 +4862,9 @@
       <c r="E15">
         <v>0</v>
       </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C16" t="s">
@@ -4426,8 +4876,11 @@
       <c r="E16">
         <v>5042</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F16">
+        <v>4478</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
         <v>0</v>
       </c>
@@ -4440,8 +4893,11 @@
       <c r="E17">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C18" t="s">
         <v>7</v>
       </c>
@@ -4451,8 +4907,11 @@
       <c r="E18">
         <v>849</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F18">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>14</v>
       </c>
@@ -4468,8 +4927,11 @@
       <c r="E19">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C20" t="s">
         <v>7</v>
       </c>
@@ -4479,8 +4941,11 @@
       <c r="E20">
         <v>20201</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F20">
+        <v>24236</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
         <v>2</v>
       </c>
@@ -4493,8 +4958,11 @@
       <c r="E21">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C22" t="s">
         <v>7</v>
       </c>
@@ -4504,8 +4972,11 @@
       <c r="E22">
         <v>10930</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F22">
+        <v>13332</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
         <v>1</v>
       </c>
@@ -4518,8 +4989,11 @@
       <c r="E23">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C24" t="s">
         <v>7</v>
       </c>
@@ -4529,8 +5003,11 @@
       <c r="E24">
         <v>5820</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F24">
+        <v>7122</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B25" t="s">
         <v>0</v>
       </c>
@@ -4543,8 +5020,11 @@
       <c r="E25">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C26" t="s">
         <v>7</v>
       </c>
@@ -4554,8 +5034,11 @@
       <c r="E26">
         <v>1006</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F26">
+        <v>763</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>13</v>
       </c>
@@ -4571,8 +5054,11 @@
       <c r="E27" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F27" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C28" t="s">
         <v>7</v>
       </c>
@@ -4582,8 +5068,11 @@
       <c r="E28" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F28" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B29" t="s">
         <v>2</v>
       </c>
@@ -4596,8 +5085,11 @@
       <c r="E29" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F29" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C30" t="s">
         <v>7</v>
       </c>
@@ -4607,8 +5099,11 @@
       <c r="E30" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F30" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B31" t="s">
         <v>1</v>
       </c>
@@ -4621,8 +5116,11 @@
       <c r="E31" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F31" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C32" t="s">
         <v>7</v>
       </c>
@@ -4632,8 +5130,11 @@
       <c r="E32" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F32" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B33" t="s">
         <v>0</v>
       </c>
@@ -4646,8 +5147,11 @@
       <c r="E33" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F33" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C34" t="s">
         <v>7</v>
       </c>
@@ -4657,8 +5161,11 @@
       <c r="E34" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F34" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>12</v>
       </c>
@@ -4674,8 +5181,11 @@
       <c r="E35" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F35" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C36" t="s">
         <v>7</v>
       </c>
@@ -4685,8 +5195,11 @@
       <c r="E36" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F36" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B37" t="s">
         <v>2</v>
       </c>
@@ -4699,8 +5212,11 @@
       <c r="E37" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F37" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C38" t="s">
         <v>7</v>
       </c>
@@ -4710,8 +5226,11 @@
       <c r="E38" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F38" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B39" t="s">
         <v>1</v>
       </c>
@@ -4724,8 +5243,11 @@
       <c r="E39" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F39" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C40" t="s">
         <v>7</v>
       </c>
@@ -4735,8 +5257,11 @@
       <c r="E40" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F40" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B41" t="s">
         <v>0</v>
       </c>
@@ -4749,8 +5274,11 @@
       <c r="E41" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F41" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C42" t="s">
         <v>7</v>
       </c>
@@ -4760,8 +5288,11 @@
       <c r="E42" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F42" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>11</v>
       </c>
@@ -4777,8 +5308,11 @@
       <c r="E43" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F43" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C44" t="s">
         <v>7</v>
       </c>
@@ -4788,8 +5322,11 @@
       <c r="E44" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F44" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B45" t="s">
         <v>2</v>
       </c>
@@ -4802,8 +5339,11 @@
       <c r="E45" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F45" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C46" t="s">
         <v>7</v>
       </c>
@@ -4813,8 +5353,11 @@
       <c r="E46" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F46" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B47" t="s">
         <v>1</v>
       </c>
@@ -4827,8 +5370,11 @@
       <c r="E47" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F47" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C48" t="s">
         <v>7</v>
       </c>
@@ -4838,8 +5384,11 @@
       <c r="E48" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F48" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B49" t="s">
         <v>0</v>
       </c>
@@ -4852,8 +5401,11 @@
       <c r="E49" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F49" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C50" t="s">
         <v>7</v>
       </c>
@@ -4863,8 +5415,11 @@
       <c r="E50" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F50" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>40</v>
       </c>
@@ -4877,8 +5432,11 @@
       <c r="E51" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F51" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B52" t="s">
         <v>2</v>
       </c>
@@ -4888,8 +5446,11 @@
       <c r="E52" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F52" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B53" t="s">
         <v>1</v>
       </c>
@@ -4899,8 +5460,11 @@
       <c r="E53" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F53" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B54" t="s">
         <v>0</v>
       </c>
@@ -4910,8 +5474,11 @@
       <c r="E54" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F54" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>10</v>
       </c>
@@ -4927,8 +5494,11 @@
       <c r="E55" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F55" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C56" t="s">
         <v>7</v>
       </c>
@@ -4938,8 +5508,11 @@
       <c r="E56" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F56" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B57" t="s">
         <v>2</v>
       </c>
@@ -4952,8 +5525,11 @@
       <c r="E57" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F57" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C58" t="s">
         <v>7</v>
       </c>
@@ -4963,8 +5539,11 @@
       <c r="E58" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F58" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B59" t="s">
         <v>1</v>
       </c>
@@ -4977,8 +5556,11 @@
       <c r="E59" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F59" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C60" t="s">
         <v>7</v>
       </c>
@@ -4988,8 +5570,11 @@
       <c r="E60" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F60" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B61" t="s">
         <v>0</v>
       </c>
@@ -5002,8 +5587,11 @@
       <c r="E61" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F61" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C62" t="s">
         <v>7</v>
       </c>
@@ -5013,8 +5601,11 @@
       <c r="E62" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F62" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>9</v>
       </c>
@@ -5030,8 +5621,11 @@
       <c r="E63" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F63" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C64" t="s">
         <v>7</v>
       </c>
@@ -5040,6 +5634,9 @@
       </c>
       <c r="E64" t="s">
         <v>91</v>
+      </c>
+      <c r="F64" t="s">
+        <v>477</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.2">
@@ -5055,6 +5652,9 @@
       <c r="E65" t="s">
         <v>92</v>
       </c>
+      <c r="F65" t="s">
+        <v>478</v>
+      </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C66" t="s">
@@ -5065,6 +5665,9 @@
       </c>
       <c r="E66" t="s">
         <v>93</v>
+      </c>
+      <c r="F66" t="s">
+        <v>479</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.2">
@@ -5080,6 +5683,9 @@
       <c r="E67" t="s">
         <v>94</v>
       </c>
+      <c r="F67" t="s">
+        <v>480</v>
+      </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C68" t="s">
@@ -5091,6 +5697,9 @@
       <c r="E68" t="s">
         <v>95</v>
       </c>
+      <c r="F68" t="s">
+        <v>481</v>
+      </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B69" t="s">
@@ -5105,6 +5714,9 @@
       <c r="E69" t="s">
         <v>96</v>
       </c>
+      <c r="F69" t="s">
+        <v>482</v>
+      </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C70" t="s">
@@ -5115,6 +5727,9 @@
       </c>
       <c r="E70" t="s">
         <v>97</v>
+      </c>
+      <c r="F70" t="s">
+        <v>483</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.2">
@@ -5126,6 +5741,9 @@
       </c>
       <c r="E71" t="s">
         <v>98</v>
+      </c>
+      <c r="F71" t="s">
+        <v>484</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.2">
@@ -5164,6 +5782,9 @@
       <c r="E74">
         <v>54271</v>
       </c>
+      <c r="F74">
+        <v>70538</v>
+      </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B75" t="s">
@@ -5175,6 +5796,9 @@
       <c r="E75">
         <v>42098</v>
       </c>
+      <c r="F75">
+        <v>55604</v>
+      </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B76" t="s">
@@ -5186,6 +5810,9 @@
       <c r="E76">
         <v>14104</v>
       </c>
+      <c r="F76">
+        <v>17444</v>
+      </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B77" t="s">
@@ -5196,6 +5823,9 @@
       </c>
       <c r="E77">
         <v>4107</v>
+      </c>
+      <c r="F77">
+        <v>5075</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.2">
@@ -5211,6 +5841,9 @@
       <c r="E78">
         <v>62782</v>
       </c>
+      <c r="F78">
+        <v>60178</v>
+      </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B79" t="s">
@@ -5222,6 +5855,9 @@
       <c r="E79">
         <v>26701</v>
       </c>
+      <c r="F79">
+        <v>26637</v>
+      </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B80" t="s">
@@ -5233,6 +5869,9 @@
       <c r="E80">
         <v>8752</v>
       </c>
+      <c r="F80">
+        <v>7861</v>
+      </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B81" t="s">
@@ -5243,6 +5882,9 @@
       </c>
       <c r="E81">
         <v>834</v>
+      </c>
+      <c r="F81">
+        <v>868</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.2">
@@ -5258,6 +5900,9 @@
       <c r="E82">
         <v>59</v>
       </c>
+      <c r="F82">
+        <v>46</v>
+      </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B83" t="s">
@@ -5269,6 +5914,9 @@
       <c r="E83">
         <v>63</v>
       </c>
+      <c r="F83">
+        <v>69</v>
+      </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B84" t="s">
@@ -5280,6 +5928,9 @@
       <c r="E84">
         <v>83</v>
       </c>
+      <c r="F84">
+        <v>70</v>
+      </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B85" t="s">
@@ -5290,6 +5941,9 @@
       </c>
       <c r="E85">
         <v>528</v>
+      </c>
+      <c r="F85">
+        <v>1825</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.2">
@@ -5305,6 +5959,9 @@
       <c r="E86" t="s">
         <v>99</v>
       </c>
+      <c r="F86" t="s">
+        <v>485</v>
+      </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B87" t="s">
@@ -5316,6 +5973,9 @@
       <c r="E87" t="s">
         <v>100</v>
       </c>
+      <c r="F87" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B88" t="s">
@@ -5327,6 +5987,9 @@
       <c r="E88" t="s">
         <v>101</v>
       </c>
+      <c r="F88" t="s">
+        <v>487</v>
+      </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B89" t="s">
@@ -5337,6 +6000,9 @@
       </c>
       <c r="E89" t="s">
         <v>102</v>
+      </c>
+      <c r="F89" t="s">
+        <v>488</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.2">
@@ -5352,6 +6018,9 @@
       <c r="E90" t="s">
         <v>103</v>
       </c>
+      <c r="F90" t="s">
+        <v>489</v>
+      </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B91" t="s">
@@ -5363,6 +6032,9 @@
       <c r="E91" t="s">
         <v>104</v>
       </c>
+      <c r="F91" t="s">
+        <v>490</v>
+      </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B92" t="s">
@@ -5374,6 +6046,9 @@
       <c r="E92" t="s">
         <v>105</v>
       </c>
+      <c r="F92" t="s">
+        <v>491</v>
+      </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B93" t="s">
@@ -5384,6 +6059,9 @@
       </c>
       <c r="E93" t="s">
         <v>106</v>
+      </c>
+      <c r="F93" t="s">
+        <v>492</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.2">
@@ -5425,8 +6103,11 @@
       <c r="E96">
         <v>153</v>
       </c>
-    </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F96">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C97" t="s">
         <v>7</v>
       </c>
@@ -5436,8 +6117,11 @@
       <c r="E97">
         <v>83034</v>
       </c>
-    </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F97">
+        <v>98558</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B98" t="s">
         <v>2</v>
       </c>
@@ -5450,8 +6134,11 @@
       <c r="E98">
         <v>115</v>
       </c>
-    </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F98">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C99" t="s">
         <v>7</v>
       </c>
@@ -5461,8 +6148,11 @@
       <c r="E99">
         <v>65823</v>
       </c>
-    </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F99">
+        <v>69604</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B100" t="s">
         <v>1</v>
       </c>
@@ -5475,8 +6165,11 @@
       <c r="E100">
         <v>55</v>
       </c>
-    </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F100">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C101" t="s">
         <v>7</v>
       </c>
@@ -5486,8 +6179,11 @@
       <c r="E101">
         <v>25233</v>
       </c>
-    </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F101">
+        <v>30884</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B102" t="s">
         <v>0</v>
       </c>
@@ -5500,8 +6196,11 @@
       <c r="E102">
         <v>14</v>
       </c>
-    </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F102">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C103" t="s">
         <v>7</v>
       </c>
@@ -5511,8 +6210,11 @@
       <c r="E103">
         <v>8912</v>
       </c>
-    </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F103">
+        <v>9363</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>19</v>
       </c>
@@ -5528,8 +6230,11 @@
       <c r="E104">
         <v>25</v>
       </c>
-    </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F104">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C105" t="s">
         <v>7</v>
       </c>
@@ -5539,8 +6244,11 @@
       <c r="E105">
         <v>12519</v>
       </c>
-    </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F105">
+        <v>14708</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B106" t="s">
         <v>2</v>
       </c>
@@ -5553,8 +6261,11 @@
       <c r="E106">
         <v>19</v>
       </c>
-    </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F106">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C107" t="s">
         <v>7</v>
       </c>
@@ -5564,8 +6275,11 @@
       <c r="E107">
         <v>9783</v>
       </c>
-    </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F107">
+        <v>10624</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B108" t="s">
         <v>1</v>
       </c>
@@ -5578,8 +6292,11 @@
       <c r="E108">
         <v>7</v>
       </c>
-    </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F108">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C109" t="s">
         <v>7</v>
       </c>
@@ -5589,8 +6306,11 @@
       <c r="E109">
         <v>3861</v>
       </c>
-    </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F109">
+        <v>4687</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B110" t="s">
         <v>0</v>
       </c>
@@ -5603,8 +6323,11 @@
       <c r="E110">
         <v>2</v>
       </c>
-    </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F110">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C111" t="s">
         <v>7</v>
       </c>
@@ -5614,8 +6337,11 @@
       <c r="E111">
         <v>1342</v>
       </c>
-    </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F111">
+        <v>1395</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>20</v>
       </c>
@@ -5624,6 +6350,9 @@
       </c>
       <c r="E112" t="s">
         <v>107</v>
+      </c>
+      <c r="F112" t="s">
+        <v>493</v>
       </c>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.2">
@@ -5659,6 +6388,9 @@
       <c r="E115">
         <v>103717</v>
       </c>
+      <c r="F115">
+        <v>93529</v>
+      </c>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
@@ -5670,6 +6402,9 @@
       <c r="E116">
         <v>7275</v>
       </c>
+      <c r="F116">
+        <v>0</v>
+      </c>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
@@ -5681,6 +6416,9 @@
       <c r="E117">
         <v>33335</v>
       </c>
+      <c r="F117">
+        <v>21894</v>
+      </c>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
@@ -5692,6 +6430,9 @@
       <c r="E118">
         <v>63107</v>
       </c>
+      <c r="F118">
+        <v>71635</v>
+      </c>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
@@ -5703,6 +6444,9 @@
       <c r="E119" t="s">
         <v>108</v>
       </c>
+      <c r="F119" t="s">
+        <v>275</v>
+      </c>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
@@ -5713,6 +6457,9 @@
       </c>
       <c r="E120" t="s">
         <v>109</v>
+      </c>
+      <c r="F120" t="s">
+        <v>494</v>
       </c>
     </row>
   </sheetData>
@@ -5731,8 +6478,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BFD2204-262E-44E1-AB55-86008F8A8FE1}">
   <dimension ref="A1:G120"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F126" sqref="F126"/>
+    <sheetView tabSelected="1" topLeftCell="A112" workbookViewId="0">
+      <selection activeCell="F121" sqref="F121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5786,6 +6533,9 @@
       <c r="E3">
         <v>218</v>
       </c>
+      <c r="F3">
+        <v>241</v>
+      </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C4" t="s">
@@ -5796,6 +6546,9 @@
       </c>
       <c r="E4">
         <v>139260</v>
+      </c>
+      <c r="F4">
+        <v>160570</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -5811,6 +6564,9 @@
       <c r="E5">
         <v>138</v>
       </c>
+      <c r="F5">
+        <v>126</v>
+      </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C6" t="s">
@@ -5821,6 +6577,9 @@
       </c>
       <c r="E6">
         <v>100181</v>
+      </c>
+      <c r="F6">
+        <v>106191</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
@@ -5836,6 +6595,9 @@
       <c r="E7">
         <v>62</v>
       </c>
+      <c r="F7">
+        <v>75</v>
+      </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C8" t="s">
@@ -5847,6 +6609,9 @@
       <c r="E8">
         <v>42196</v>
       </c>
+      <c r="F8">
+        <v>49835</v>
+      </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
@@ -5861,6 +6626,9 @@
       <c r="E9">
         <v>27</v>
       </c>
+      <c r="F9">
+        <v>27</v>
+      </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C10" t="s">
@@ -5871,6 +6639,9 @@
       </c>
       <c r="E10">
         <v>12819</v>
+      </c>
+      <c r="F10">
+        <v>12623</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
@@ -5889,6 +6660,9 @@
       <c r="E11">
         <v>1</v>
       </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C12" t="s">
@@ -5899,6 +6673,9 @@
       </c>
       <c r="E12">
         <v>16771</v>
+      </c>
+      <c r="F12">
+        <v>15192</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
@@ -5914,6 +6691,9 @@
       <c r="E13">
         <v>0</v>
       </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C14" t="s">
@@ -5924,6 +6704,9 @@
       </c>
       <c r="E14">
         <v>8548</v>
+      </c>
+      <c r="F14">
+        <v>7352</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
@@ -5939,6 +6722,9 @@
       <c r="E15">
         <v>0</v>
       </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C16" t="s">
@@ -5950,8 +6736,11 @@
       <c r="E16">
         <v>5278</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F16">
+        <v>4668</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
         <v>0</v>
       </c>
@@ -5964,8 +6753,11 @@
       <c r="E17">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C18" t="s">
         <v>7</v>
       </c>
@@ -5975,8 +6767,11 @@
       <c r="E18">
         <v>1045</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F18">
+        <v>631</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>14</v>
       </c>
@@ -5992,8 +6787,11 @@
       <c r="E19">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C20" t="s">
         <v>7</v>
       </c>
@@ -6003,8 +6801,11 @@
       <c r="E20">
         <v>21602</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F20">
+        <v>25354</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
         <v>2</v>
       </c>
@@ -6017,8 +6818,11 @@
       <c r="E21">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C22" t="s">
         <v>7</v>
       </c>
@@ -6028,8 +6832,11 @@
       <c r="E22">
         <v>11495</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F22">
+        <v>13964</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
         <v>1</v>
       </c>
@@ -6042,8 +6849,11 @@
       <c r="E23">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C24" t="s">
         <v>7</v>
       </c>
@@ -6053,8 +6863,11 @@
       <c r="E24">
         <v>6169</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F24">
+        <v>7449</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B25" t="s">
         <v>0</v>
       </c>
@@ -6067,8 +6880,11 @@
       <c r="E25">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C26" t="s">
         <v>7</v>
       </c>
@@ -6078,8 +6894,11 @@
       <c r="E26">
         <v>1241</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F26">
+        <v>1287</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>13</v>
       </c>
@@ -6095,8 +6914,11 @@
       <c r="E27" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F27" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C28" t="s">
         <v>7</v>
       </c>
@@ -6106,8 +6928,11 @@
       <c r="E28" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F28" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B29" t="s">
         <v>2</v>
       </c>
@@ -6120,8 +6945,11 @@
       <c r="E29" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F29" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C30" t="s">
         <v>7</v>
       </c>
@@ -6131,8 +6959,11 @@
       <c r="E30" t="s">
         <v>219</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F30" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B31" t="s">
         <v>1</v>
       </c>
@@ -6145,8 +6976,11 @@
       <c r="E31" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F31" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C32" t="s">
         <v>7</v>
       </c>
@@ -6156,8 +6990,11 @@
       <c r="E32" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F32" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B33" t="s">
         <v>0</v>
       </c>
@@ -6170,8 +7007,11 @@
       <c r="E33" t="s">
         <v>222</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F33" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C34" t="s">
         <v>7</v>
       </c>
@@ -6181,8 +7021,11 @@
       <c r="E34" t="s">
         <v>223</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F34" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>12</v>
       </c>
@@ -6198,8 +7041,11 @@
       <c r="E35" t="s">
         <v>224</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F35" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C36" t="s">
         <v>7</v>
       </c>
@@ -6209,8 +7055,11 @@
       <c r="E36" t="s">
         <v>225</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F36" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B37" t="s">
         <v>2</v>
       </c>
@@ -6223,8 +7072,11 @@
       <c r="E37" t="s">
         <v>226</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F37" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C38" t="s">
         <v>7</v>
       </c>
@@ -6234,8 +7086,11 @@
       <c r="E38" t="s">
         <v>227</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F38" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B39" t="s">
         <v>1</v>
       </c>
@@ -6248,8 +7103,11 @@
       <c r="E39" t="s">
         <v>228</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F39" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C40" t="s">
         <v>7</v>
       </c>
@@ -6259,8 +7117,11 @@
       <c r="E40" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F40" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B41" t="s">
         <v>0</v>
       </c>
@@ -6273,8 +7134,11 @@
       <c r="E41" t="s">
         <v>230</v>
       </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F41" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C42" t="s">
         <v>7</v>
       </c>
@@ -6284,8 +7148,11 @@
       <c r="E42" t="s">
         <v>231</v>
       </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F42" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>11</v>
       </c>
@@ -6301,8 +7168,11 @@
       <c r="E43" t="s">
         <v>232</v>
       </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F43" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C44" t="s">
         <v>7</v>
       </c>
@@ -6312,8 +7182,11 @@
       <c r="E44" t="s">
         <v>233</v>
       </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F44" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B45" t="s">
         <v>2</v>
       </c>
@@ -6326,8 +7199,11 @@
       <c r="E45" t="s">
         <v>234</v>
       </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F45" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C46" t="s">
         <v>7</v>
       </c>
@@ -6337,8 +7213,11 @@
       <c r="E46" t="s">
         <v>235</v>
       </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F46" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B47" t="s">
         <v>1</v>
       </c>
@@ -6351,8 +7230,11 @@
       <c r="E47" t="s">
         <v>236</v>
       </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F47" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C48" t="s">
         <v>7</v>
       </c>
@@ -6362,8 +7244,11 @@
       <c r="E48" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F48" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B49" t="s">
         <v>0</v>
       </c>
@@ -6376,8 +7261,11 @@
       <c r="E49" t="s">
         <v>238</v>
       </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F49" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C50" t="s">
         <v>7</v>
       </c>
@@ -6387,8 +7275,11 @@
       <c r="E50" t="s">
         <v>239</v>
       </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F50" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>40</v>
       </c>
@@ -6401,8 +7292,11 @@
       <c r="E51" t="s">
         <v>240</v>
       </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F51" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B52" t="s">
         <v>2</v>
       </c>
@@ -6412,8 +7306,11 @@
       <c r="E52" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F52" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B53" t="s">
         <v>1</v>
       </c>
@@ -6423,8 +7320,11 @@
       <c r="E53" t="s">
         <v>242</v>
       </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F53" t="s">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B54" t="s">
         <v>0</v>
       </c>
@@ -6434,8 +7334,11 @@
       <c r="E54" t="s">
         <v>243</v>
       </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F54" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>10</v>
       </c>
@@ -6451,8 +7354,11 @@
       <c r="E55" t="s">
         <v>244</v>
       </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F55" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C56" t="s">
         <v>7</v>
       </c>
@@ -6462,8 +7368,11 @@
       <c r="E56" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F56" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B57" t="s">
         <v>2</v>
       </c>
@@ -6476,8 +7385,11 @@
       <c r="E57" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F57" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C58" t="s">
         <v>7</v>
       </c>
@@ -6487,8 +7399,11 @@
       <c r="E58" t="s">
         <v>247</v>
       </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F58" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B59" t="s">
         <v>1</v>
       </c>
@@ -6501,8 +7416,11 @@
       <c r="E59" t="s">
         <v>248</v>
       </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F59" t="s">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C60" t="s">
         <v>7</v>
       </c>
@@ -6512,8 +7430,11 @@
       <c r="E60" t="s">
         <v>249</v>
       </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F60" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B61" t="s">
         <v>0</v>
       </c>
@@ -6526,8 +7447,11 @@
       <c r="E61" t="s">
         <v>250</v>
       </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F61" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C62" t="s">
         <v>7</v>
       </c>
@@ -6537,8 +7461,11 @@
       <c r="E62" t="s">
         <v>251</v>
       </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F62" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>9</v>
       </c>
@@ -6554,8 +7481,11 @@
       <c r="E63" t="s">
         <v>252</v>
       </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F63" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C64" t="s">
         <v>7</v>
       </c>
@@ -6564,6 +7494,9 @@
       </c>
       <c r="E64" t="s">
         <v>253</v>
+      </c>
+      <c r="F64" t="s">
+        <v>531</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.2">
@@ -6579,6 +7512,9 @@
       <c r="E65" t="s">
         <v>254</v>
       </c>
+      <c r="F65" t="s">
+        <v>532</v>
+      </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C66" t="s">
@@ -6589,6 +7525,9 @@
       </c>
       <c r="E66" t="s">
         <v>255</v>
+      </c>
+      <c r="F66" t="s">
+        <v>533</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.2">
@@ -6604,6 +7543,9 @@
       <c r="E67" t="s">
         <v>256</v>
       </c>
+      <c r="F67" t="s">
+        <v>272</v>
+      </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C68" t="s">
@@ -6615,6 +7557,9 @@
       <c r="E68" t="s">
         <v>257</v>
       </c>
+      <c r="F68" t="s">
+        <v>534</v>
+      </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B69" t="s">
@@ -6629,6 +7574,9 @@
       <c r="E69" t="s">
         <v>258</v>
       </c>
+      <c r="F69" t="s">
+        <v>535</v>
+      </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C70" t="s">
@@ -6639,6 +7587,9 @@
       </c>
       <c r="E70" t="s">
         <v>259</v>
+      </c>
+      <c r="F70" t="s">
+        <v>536</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.2">
@@ -6650,6 +7601,9 @@
       </c>
       <c r="E71" t="s">
         <v>98</v>
+      </c>
+      <c r="F71" t="s">
+        <v>537</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.2">
@@ -6688,6 +7642,9 @@
       <c r="E74">
         <v>58910</v>
       </c>
+      <c r="F74">
+        <v>75728</v>
+      </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B75" t="s">
@@ -6699,6 +7656,9 @@
       <c r="E75">
         <v>45817</v>
       </c>
+      <c r="F75">
+        <v>59617</v>
+      </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B76" t="s">
@@ -6710,6 +7670,9 @@
       <c r="E76">
         <v>15266</v>
       </c>
+      <c r="F76">
+        <v>18743</v>
+      </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B77" t="s">
@@ -6720,6 +7683,9 @@
       </c>
       <c r="E77">
         <v>4457</v>
+      </c>
+      <c r="F77">
+        <v>5415</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.2">
@@ -6735,6 +7701,9 @@
       <c r="E78">
         <v>65395</v>
       </c>
+      <c r="F78">
+        <v>62546</v>
+      </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B79" t="s">
@@ -6746,6 +7715,9 @@
       <c r="E79">
         <v>27836</v>
       </c>
+      <c r="F79">
+        <v>28549</v>
+      </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B80" t="s">
@@ -6757,6 +7729,9 @@
       <c r="E80">
         <v>9068</v>
       </c>
+      <c r="F80">
+        <v>8520</v>
+      </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B81" t="s">
@@ -6767,6 +7742,9 @@
       </c>
       <c r="E81">
         <v>1045</v>
+      </c>
+      <c r="F81">
+        <v>1442</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.2">
@@ -6782,6 +7760,9 @@
       <c r="E82">
         <v>264</v>
       </c>
+      <c r="F82">
+        <v>211</v>
+      </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B83" t="s">
@@ -6793,6 +7774,9 @@
       <c r="E83">
         <v>233</v>
       </c>
+      <c r="F83">
+        <v>242</v>
+      </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B84" t="s">
@@ -6804,6 +7788,9 @@
       <c r="E84">
         <v>274</v>
       </c>
+      <c r="F84">
+        <v>200</v>
+      </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B85" t="s">
@@ -6814,6 +7801,9 @@
       </c>
       <c r="E85">
         <v>177</v>
+      </c>
+      <c r="F85">
+        <v>156</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.2">
@@ -6829,6 +7819,9 @@
       <c r="E86" t="s">
         <v>260</v>
       </c>
+      <c r="F86" t="s">
+        <v>538</v>
+      </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B87" t="s">
@@ -6840,6 +7833,9 @@
       <c r="E87" t="s">
         <v>261</v>
       </c>
+      <c r="F87" t="s">
+        <v>539</v>
+      </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B88" t="s">
@@ -6851,6 +7847,9 @@
       <c r="E88" t="s">
         <v>262</v>
       </c>
+      <c r="F88" t="s">
+        <v>540</v>
+      </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B89" t="s">
@@ -6861,6 +7860,9 @@
       </c>
       <c r="E89" t="s">
         <v>263</v>
+      </c>
+      <c r="F89" t="s">
+        <v>541</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.2">
@@ -6876,6 +7878,9 @@
       <c r="E90" t="s">
         <v>264</v>
       </c>
+      <c r="F90" t="s">
+        <v>542</v>
+      </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B91" t="s">
@@ -6887,6 +7892,9 @@
       <c r="E91" t="s">
         <v>265</v>
       </c>
+      <c r="F91" t="s">
+        <v>543</v>
+      </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B92" t="s">
@@ -6898,6 +7906,9 @@
       <c r="E92" t="s">
         <v>266</v>
       </c>
+      <c r="F92" t="s">
+        <v>544</v>
+      </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B93" t="s">
@@ -6908,6 +7919,9 @@
       </c>
       <c r="E93" t="s">
         <v>267</v>
+      </c>
+      <c r="F93" t="s">
+        <v>545</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.2">
@@ -6949,6 +7963,9 @@
       <c r="E96">
         <v>171</v>
       </c>
+      <c r="F96">
+        <v>195</v>
+      </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C97" t="s">
@@ -6959,6 +7976,9 @@
       </c>
       <c r="E97">
         <v>81164</v>
+      </c>
+      <c r="F97">
+        <v>96753</v>
       </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.2">
@@ -6974,6 +7994,9 @@
       <c r="E98">
         <v>113</v>
       </c>
+      <c r="F98">
+        <v>100</v>
+      </c>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C99" t="s">
@@ -6984,6 +8007,9 @@
       </c>
       <c r="E99">
         <v>64937</v>
+      </c>
+      <c r="F99">
+        <v>68550</v>
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.2">
@@ -6999,6 +8025,9 @@
       <c r="E100">
         <v>47</v>
       </c>
+      <c r="F100">
+        <v>62</v>
+      </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C101" t="s">
@@ -7010,6 +8039,9 @@
       <c r="E101">
         <v>24672</v>
       </c>
+      <c r="F101">
+        <v>30274</v>
+      </c>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B102" t="s">
@@ -7024,6 +8056,9 @@
       <c r="E102">
         <v>22</v>
       </c>
+      <c r="F102">
+        <v>25</v>
+      </c>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C103" t="s">
@@ -7034,6 +8069,9 @@
       </c>
       <c r="E103">
         <v>8491</v>
+      </c>
+      <c r="F103">
+        <v>8630</v>
       </c>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.2">
@@ -7052,6 +8090,9 @@
       <c r="E104">
         <v>46</v>
       </c>
+      <c r="F104">
+        <v>46</v>
+      </c>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C105" t="s">
@@ -7062,6 +8103,9 @@
       </c>
       <c r="E105">
         <v>19792</v>
+      </c>
+      <c r="F105">
+        <v>23513</v>
       </c>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.2">
@@ -7077,6 +8121,9 @@
       <c r="E106">
         <v>25</v>
       </c>
+      <c r="F106">
+        <v>26</v>
+      </c>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C107" t="s">
@@ -7087,6 +8134,9 @@
       </c>
       <c r="E107">
         <v>15535</v>
+      </c>
+      <c r="F107">
+        <v>16550</v>
       </c>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.2">
@@ -7102,6 +8152,9 @@
       <c r="E108">
         <v>15</v>
       </c>
+      <c r="F108">
+        <v>13</v>
+      </c>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C109" t="s">
@@ -7113,6 +8166,9 @@
       <c r="E109">
         <v>6078</v>
       </c>
+      <c r="F109">
+        <v>7479</v>
+      </c>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B110" t="s">
@@ -7127,6 +8183,9 @@
       <c r="E110">
         <v>5</v>
       </c>
+      <c r="F110">
+        <v>2</v>
+      </c>
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C111" t="s">
@@ -7137,6 +8196,9 @@
       </c>
       <c r="E111">
         <v>2109</v>
+      </c>
+      <c r="F111">
+        <v>2097</v>
       </c>
       <c r="G111" s="9"/>
     </row>
@@ -7149,6 +8211,9 @@
       </c>
       <c r="E112" t="s">
         <v>268</v>
+      </c>
+      <c r="F112" t="s">
+        <v>546</v>
       </c>
       <c r="G112" s="9"/>
     </row>
@@ -7185,6 +8250,9 @@
       <c r="E115">
         <v>103717</v>
       </c>
+      <c r="F115">
+        <v>93529</v>
+      </c>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
@@ -7196,6 +8264,9 @@
       <c r="E116">
         <v>7437</v>
       </c>
+      <c r="F116">
+        <v>0</v>
+      </c>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
@@ -7207,6 +8278,9 @@
       <c r="E117">
         <v>33288</v>
       </c>
+      <c r="F117">
+        <v>21894</v>
+      </c>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
@@ -7218,6 +8292,9 @@
       <c r="E118">
         <v>62992</v>
       </c>
+      <c r="F118">
+        <v>71635</v>
+      </c>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
@@ -7229,6 +8306,9 @@
       <c r="E119" t="s">
         <v>269</v>
       </c>
+      <c r="F119" t="s">
+        <v>275</v>
+      </c>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
@@ -7239,6 +8319,9 @@
       </c>
       <c r="E120" t="s">
         <v>270</v>
+      </c>
+      <c r="F120" t="s">
+        <v>547</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added scipt to be completed
</commit_message>
<xml_diff>
--- a/data/CONFRONTO_VERSIONI.xlsx
+++ b/data/CONFRONTO_VERSIONI.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uniroma2-my.sharepoint.com/personal/livia_simoncini_alumni_uniroma2_eu/Documents/Corsi/Attivi/PMCSN/Progetto/PMCSN_Project/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oem\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="108" documentId="13_ncr:1_{79D3C2E9-C11C-408C-9918-E7BCF1F966EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9E13400F-7AB4-429D-A945-EC0AD23E91A9}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1E5C654-0C66-42AF-AE99-454FDD4F7F0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{58870B00-CDA7-45B2-A026-0B544E698EBB}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{58870B00-CDA7-45B2-A026-0B544E698EBB}"/>
   </bookViews>
   <sheets>
     <sheet name="Analytical" sheetId="12" r:id="rId1"/>
@@ -39,32 +39,8 @@
 </workbook>
 </file>
 
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author>oem</author>
-  </authors>
-  <commentList>
-    <comment ref="A27" authorId="0" shapeId="0" xr:uid="{2D378857-45E0-4C16-8BC3-B927A9C0B480}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">Computed as:
-- </t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1320" uniqueCount="550">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1327" uniqueCount="553">
   <si>
     <t>AB</t>
   </si>
@@ -1710,10 +1686,19 @@
     <t>42.779000,+/-1.372047</t>
   </si>
   <si>
-    <t>V1</t>
-  </si>
-  <si>
-    <t>V3</t>
+    <t>V2 - 2019</t>
+  </si>
+  <si>
+    <t>V1 - avg(2014/2019)</t>
+  </si>
+  <si>
+    <t>V3 - sum(2010/2019)</t>
+  </si>
+  <si>
+    <t>V1 - avg(2014/2019) * 10y</t>
+  </si>
+  <si>
+    <t>V2 - 2019 * 10y</t>
   </si>
 </sst>
 </file>
@@ -1753,9 +1738,9 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
+      <sz val="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
       <charset val="1"/>
     </font>
   </fonts>
@@ -1859,7 +1844,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1878,14 +1863,19 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
@@ -1902,10 +1892,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2205,40 +2191,49 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD5C38B3-49E9-458D-8669-DF8830114E35}">
-  <dimension ref="A1:E112"/>
+  <dimension ref="A1:F112"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K120" sqref="K120"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="H43" sqref="H43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="43" customWidth="1"/>
-    <col min="4" max="4" width="13.5703125" customWidth="1"/>
+    <col min="4" max="4" width="23" customWidth="1"/>
     <col min="5" max="5" width="15.85546875" customWidth="1"/>
+    <col min="6" max="6" width="19" customWidth="1"/>
+    <col min="8" max="8" width="24" customWidth="1"/>
+    <col min="9" max="9" width="23.42578125" customWidth="1"/>
+    <col min="10" max="10" width="21.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="19" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" s="18" t="s">
         <v>38</v>
       </c>
       <c r="B1" s="19"/>
       <c r="C1" s="19"/>
       <c r="D1" s="19"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+      <c r="E1" s="11"/>
+      <c r="F1" s="16"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
         <v>17</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>549</v>
+      </c>
+      <c r="E2" s="15" t="s">
         <v>548</v>
       </c>
-      <c r="E2" s="15" t="s">
-        <v>549</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="F2" s="17" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="5" t="s">
         <v>16</v>
       </c>
       <c r="B3" t="s">
@@ -2247,53 +2242,132 @@
       <c r="C3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D3">
+        <v>190</v>
+      </c>
+      <c r="E3">
+        <v>190</v>
+      </c>
+      <c r="F3" s="4">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="5"/>
       <c r="C4" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D4">
+        <v>137533.33333333334</v>
+      </c>
+      <c r="E4">
+        <v>153820</v>
+      </c>
+      <c r="F4" s="4">
+        <v>129759</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="5"/>
       <c r="B5" t="s">
         <v>2</v>
       </c>
       <c r="C5" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D5">
+        <v>106.66666666666666</v>
+      </c>
+      <c r="E5">
+        <v>100</v>
+      </c>
+      <c r="F5" s="4">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="5"/>
       <c r="C6" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D6">
+        <v>90031.666666666657</v>
+      </c>
+      <c r="E6">
+        <v>99150</v>
+      </c>
+      <c r="F6" s="4">
+        <v>86128</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="5"/>
       <c r="B7" t="s">
         <v>1</v>
       </c>
       <c r="C7" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D7">
+        <v>60</v>
+      </c>
+      <c r="E7">
+        <v>100</v>
+      </c>
+      <c r="F7" s="4">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" s="5"/>
       <c r="C8" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D8">
+        <v>41980</v>
+      </c>
+      <c r="E8">
+        <v>46889.999999999993</v>
+      </c>
+      <c r="F8" s="4">
+        <v>39344</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" s="5"/>
       <c r="B9" t="s">
         <v>0</v>
       </c>
       <c r="C9" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D9">
+        <v>16.666666666666668</v>
+      </c>
+      <c r="E9">
+        <v>20</v>
+      </c>
+      <c r="F9" s="4">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" s="5"/>
       <c r="C10" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+      <c r="D10">
+        <v>10511.666666666668</v>
+      </c>
+      <c r="E10">
+        <v>11600</v>
+      </c>
+      <c r="F10" s="4">
+        <v>9920</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" s="5" t="s">
         <v>15</v>
       </c>
       <c r="B11" t="s">
@@ -2302,53 +2376,132 @@
       <c r="C11" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D11">
+        <v>10</v>
+      </c>
+      <c r="E11">
+        <v>10</v>
+      </c>
+      <c r="F11" s="4">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" s="5"/>
       <c r="C12" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D12">
+        <v>9138.3333333333339</v>
+      </c>
+      <c r="E12">
+        <v>8740</v>
+      </c>
+      <c r="F12" s="4">
+        <v>9383</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" s="5"/>
       <c r="B13" t="s">
         <v>2</v>
       </c>
       <c r="C13" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D13">
+        <v>3.333333333333333</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13" s="4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" s="5"/>
       <c r="C14" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D14">
+        <v>4455</v>
+      </c>
+      <c r="E14">
+        <v>3680.0000000000005</v>
+      </c>
+      <c r="F14" s="4">
+        <v>4695</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" s="5"/>
       <c r="B15" t="s">
         <v>1</v>
       </c>
       <c r="C15" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" s="5"/>
       <c r="C16" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D16">
+        <v>2831.666666666667</v>
+      </c>
+      <c r="E16">
+        <v>2699.9999999999995</v>
+      </c>
+      <c r="F16" s="4">
+        <v>2856</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" s="5"/>
       <c r="B17" t="s">
         <v>0</v>
       </c>
       <c r="C17" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="F17" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" s="5"/>
       <c r="C18" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
+      <c r="D18">
+        <v>385</v>
+      </c>
+      <c r="E18">
+        <v>340</v>
+      </c>
+      <c r="F18" s="4">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19" s="5" t="s">
         <v>14</v>
       </c>
       <c r="B19" t="s">
@@ -2357,53 +2510,132 @@
       <c r="C19" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D19">
+        <v>23.333333333333336</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
+      <c r="F19" s="4">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20" s="5"/>
       <c r="C20" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D20">
+        <v>15215</v>
+      </c>
+      <c r="E20">
+        <v>15639.999999999998</v>
+      </c>
+      <c r="F20" s="4">
+        <v>14395</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21" s="5"/>
       <c r="B21" t="s">
         <v>2</v>
       </c>
       <c r="C21" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D21">
+        <v>5</v>
+      </c>
+      <c r="E21">
+        <v>20</v>
+      </c>
+      <c r="F21" s="4">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22" s="5"/>
       <c r="C22" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D22">
+        <v>8533.3333333333339</v>
+      </c>
+      <c r="E22">
+        <v>8640</v>
+      </c>
+      <c r="F22" s="4">
+        <v>8187</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A23" s="5"/>
       <c r="B23" t="s">
         <v>1</v>
       </c>
       <c r="C23" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D23">
+        <v>0</v>
+      </c>
+      <c r="E23">
+        <v>0</v>
+      </c>
+      <c r="F23" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A24" s="5"/>
       <c r="C24" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D24">
+        <v>4540</v>
+      </c>
+      <c r="E24">
+        <v>4780</v>
+      </c>
+      <c r="F24" s="4">
+        <v>4307</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A25" s="5"/>
       <c r="B25" t="s">
         <v>0</v>
       </c>
       <c r="C25" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D25">
+        <v>5</v>
+      </c>
+      <c r="E25">
+        <v>0</v>
+      </c>
+      <c r="F25" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A26" s="5"/>
       <c r="C26" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
+      <c r="D26">
+        <v>770</v>
+      </c>
+      <c r="E26">
+        <v>869.99999999999989</v>
+      </c>
+      <c r="F26" s="4">
+        <v>761</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A27" s="5" t="s">
         <v>13</v>
       </c>
       <c r="B27" t="s">
@@ -2415,16 +2647,30 @@
       <c r="D27">
         <v>19.210526315789451</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E27">
+        <v>19.210526315789473</v>
+      </c>
+      <c r="F27" s="4">
+        <v>20.391061452513966</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A28" s="5"/>
       <c r="C28" t="s">
         <v>7</v>
       </c>
       <c r="D28">
         <v>2.6539020843431863E-2</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E28">
+        <v>2.372903393576908E-2</v>
+      </c>
+      <c r="F28" s="4">
+        <v>2.8129070045237708E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A29" s="5"/>
       <c r="B29" t="s">
         <v>2</v>
       </c>
@@ -2434,16 +2680,30 @@
       <c r="D29">
         <v>34.21875000000005</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E29">
+        <v>36.5</v>
+      </c>
+      <c r="F29" s="4">
+        <v>36.5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A30" s="5"/>
       <c r="C30" t="s">
         <v>7</v>
       </c>
       <c r="D30">
         <v>4.0541291027231155E-2</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E30">
+        <v>3.6812909732728188E-2</v>
+      </c>
+      <c r="F30" s="4">
+        <v>4.2378785064090659E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A31" s="5"/>
       <c r="B31" t="s">
         <v>1</v>
       </c>
@@ -2453,16 +2713,30 @@
       <c r="D31">
         <v>60.833333333333186</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E31">
+        <v>36.5</v>
+      </c>
+      <c r="F31" s="4">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A32" s="5"/>
       <c r="C32" t="s">
         <v>7</v>
       </c>
       <c r="D32">
         <v>8.6946164840400186E-2</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E32">
+        <v>7.7841757304329282E-2</v>
+      </c>
+      <c r="F32" s="4">
+        <v>9.2771451809678732E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A33" s="5"/>
       <c r="B33" t="s">
         <v>0</v>
       </c>
@@ -2472,17 +2746,30 @@
       <c r="D33">
         <v>219</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E33">
+        <v>182.5</v>
+      </c>
+      <c r="F33" s="4">
+        <v>243.33333333333337</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A34" s="5"/>
       <c r="C34" t="s">
         <v>7</v>
       </c>
       <c r="D34">
         <v>0.34723323291580743</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
+      <c r="E34">
+        <v>0.31465517241379309</v>
+      </c>
+      <c r="F34" s="4">
+        <v>0.36794354838709681</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A35" s="5" t="s">
         <v>12</v>
       </c>
       <c r="B35" t="s">
@@ -2491,53 +2778,68 @@
       <c r="C35" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F35" s="4"/>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A36" s="5"/>
       <c r="C36" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F36" s="4"/>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A37" s="5"/>
       <c r="B37" t="s">
         <v>2</v>
       </c>
       <c r="C37" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F37" s="4"/>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A38" s="5"/>
       <c r="C38" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F38" s="4"/>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A39" s="5"/>
       <c r="B39" t="s">
         <v>1</v>
       </c>
       <c r="C39" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F39" s="4"/>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A40" s="5"/>
       <c r="C40" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F40" s="4"/>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A41" s="5"/>
       <c r="B41" t="s">
         <v>0</v>
       </c>
       <c r="C41" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F41" s="4"/>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A42" s="5"/>
       <c r="C42" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
+      <c r="F42" s="4"/>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A43" s="5" t="s">
         <v>11</v>
       </c>
       <c r="B43" t="s">
@@ -2546,76 +2848,98 @@
       <c r="C43" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F43" s="4"/>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A44" s="5"/>
       <c r="C44" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F44" s="4"/>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A45" s="5"/>
       <c r="B45" t="s">
         <v>2</v>
       </c>
       <c r="C45" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F45" s="4"/>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A46" s="5"/>
       <c r="C46" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F46" s="4"/>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A47" s="5"/>
       <c r="B47" t="s">
         <v>1</v>
       </c>
       <c r="C47" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F47" s="4"/>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A48" s="5"/>
       <c r="C48" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="F48" s="4"/>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A49" s="5"/>
       <c r="B49" t="s">
         <v>0</v>
       </c>
       <c r="C49" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="F49" s="4"/>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A50" s="5"/>
       <c r="C50" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A51" t="s">
+      <c r="F50" s="4"/>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A51" s="5" t="s">
         <v>40</v>
       </c>
       <c r="B51" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="F51" s="4"/>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A52" s="5"/>
       <c r="B52" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="F52" s="4"/>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A53" s="5"/>
       <c r="B53" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="F53" s="4"/>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A54" s="5"/>
       <c r="B54" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A55" t="s">
+      <c r="F54" s="4"/>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A55" s="5" t="s">
         <v>10</v>
       </c>
       <c r="B55" t="s">
@@ -2624,53 +2948,68 @@
       <c r="C55" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="F55" s="4"/>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A56" s="5"/>
       <c r="C56" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="F56" s="4"/>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A57" s="5"/>
       <c r="B57" t="s">
         <v>2</v>
       </c>
       <c r="C57" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="F57" s="4"/>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A58" s="5"/>
       <c r="C58" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="F58" s="4"/>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A59" s="5"/>
       <c r="B59" t="s">
         <v>1</v>
       </c>
       <c r="C59" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="F59" s="4"/>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A60" s="5"/>
       <c r="C60" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="F60" s="4"/>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A61" s="5"/>
       <c r="B61" t="s">
         <v>0</v>
       </c>
       <c r="C61" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="F61" s="4"/>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A62" s="5"/>
       <c r="C62" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A63" t="s">
+      <c r="F62" s="4"/>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A63" s="5" t="s">
         <v>9</v>
       </c>
       <c r="B63" t="s">
@@ -2679,119 +3018,217 @@
       <c r="C63" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="F63" s="4"/>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A64" s="5"/>
       <c r="C64" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F64" s="4"/>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A65" s="5"/>
       <c r="B65" t="s">
         <v>2</v>
       </c>
       <c r="C65" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F65" s="4"/>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A66" s="5"/>
       <c r="C66" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F66" s="4"/>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A67" s="5"/>
       <c r="B67" t="s">
         <v>1</v>
       </c>
       <c r="C67" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F67" s="4"/>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A68" s="5"/>
       <c r="C68" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F68" s="4"/>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A69" s="5"/>
       <c r="B69" t="s">
         <v>0</v>
       </c>
       <c r="C69" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F69" s="4"/>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A70" s="5"/>
       <c r="C70" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A71" t="s">
+      <c r="F70" s="4"/>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A71" s="6" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A72" s="19" t="s">
+      <c r="B71" s="7"/>
+      <c r="C71" s="7"/>
+      <c r="D71" s="7"/>
+      <c r="E71" s="7"/>
+      <c r="F71" s="8"/>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A72" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="B72" s="19"/>
-      <c r="C72" s="19"/>
-      <c r="D72" s="19"/>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B72" s="20"/>
+      <c r="C72" s="20"/>
+      <c r="D72" s="20"/>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>548</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
+        <v>551</v>
+      </c>
+      <c r="E73" s="15" t="s">
+        <v>552</v>
+      </c>
+      <c r="F73" s="17" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>48</v>
       </c>
       <c r="B74" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D74">
+        <v>44190</v>
+      </c>
+      <c r="E74">
+        <v>53220</v>
+      </c>
+      <c r="F74">
+        <v>40606</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B75" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D75">
+        <v>34305.000000000007</v>
+      </c>
+      <c r="E75">
+        <v>41270</v>
+      </c>
+      <c r="F75">
+        <v>31517</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B76" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D76">
+        <v>10905</v>
+      </c>
+      <c r="E76">
+        <v>13130</v>
+      </c>
+      <c r="F76">
+        <v>10137</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B77" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D77">
+        <v>3181.666666666667</v>
+      </c>
+      <c r="E77">
+        <v>3900</v>
+      </c>
+      <c r="F77">
+        <v>2933</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>49</v>
       </c>
       <c r="B78" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D78">
+        <v>37613.333333333336</v>
+      </c>
+      <c r="E78">
+        <v>43030</v>
+      </c>
+      <c r="F78">
+        <v>37426</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B79" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D79">
+        <v>16570</v>
+      </c>
+      <c r="E79">
+        <v>18890</v>
+      </c>
+      <c r="F79">
+        <v>16267</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B80" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D80">
+        <v>4878.3333333333339</v>
+      </c>
+      <c r="E80">
+        <v>5620</v>
+      </c>
+      <c r="F80">
+        <v>4872</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B81" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D81">
+        <v>798.33333333333337</v>
+      </c>
+      <c r="E81">
+        <v>1120</v>
+      </c>
+      <c r="F81">
+        <v>755</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>6</v>
       </c>
@@ -2799,22 +3236,22 @@
         <v>3</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B83" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B84" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B85" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>5</v>
       </c>
@@ -2824,32 +3261,56 @@
       <c r="D86">
         <v>8.2597872821905366E-2</v>
       </c>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E86">
+        <v>6.8583239383690348E-2</v>
+      </c>
+      <c r="F86">
+        <v>8.9888193862975918E-2</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B87" t="s">
         <v>2</v>
       </c>
       <c r="D87">
         <v>0.10639848418597873</v>
       </c>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E87">
+        <v>8.8441967530894117E-2</v>
+      </c>
+      <c r="F87">
+        <v>0.11581051496018022</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B88" t="s">
         <v>1</v>
       </c>
       <c r="D88">
         <v>0.33470884915176552</v>
       </c>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E88">
+        <v>0.27798933739527798</v>
+      </c>
+      <c r="F88">
+        <v>0.36006708099043111</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B89" t="s">
         <v>0</v>
       </c>
       <c r="D89">
         <v>1.1471974855945521</v>
       </c>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E89">
+        <v>0.9358974358974359</v>
+      </c>
+      <c r="F89">
+        <v>1.2444595976815547</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>4</v>
       </c>
@@ -2857,38 +3318,44 @@
         <v>3</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B91" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B92" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B93" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A94" s="19" t="s">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A94" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="B94" s="19"/>
-      <c r="C94" s="19"/>
-      <c r="D94" s="19"/>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B94" s="20"/>
+      <c r="C94" s="20"/>
+      <c r="D94" s="20"/>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A95" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D95" s="1" t="s">
+        <v>549</v>
+      </c>
+      <c r="E95" s="15" t="s">
         <v>548</v>
       </c>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F95" s="17" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>36</v>
       </c>
@@ -2899,12 +3366,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C97" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B98" t="s">
         <v>2</v>
       </c>
@@ -2912,12 +3379,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C99" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B100" t="s">
         <v>1</v>
       </c>
@@ -2925,12 +3392,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C101" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B102" t="s">
         <v>0</v>
       </c>
@@ -2938,76 +3405,103 @@
         <v>8</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C103" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A105" s="19" t="s">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A105" s="18" t="s">
         <v>30</v>
       </c>
       <c r="B105" s="19"/>
       <c r="C105" s="19"/>
       <c r="D105" s="19"/>
-    </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A106" s="1" t="s">
+      <c r="E105" s="11"/>
+      <c r="F105" s="16"/>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A106" s="2" t="s">
         <v>17</v>
       </c>
       <c r="D106" s="1" t="s">
+        <v>549</v>
+      </c>
+      <c r="E106" s="15" t="s">
         <v>548</v>
       </c>
-    </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A107" t="s">
+      <c r="F106" s="17" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A107" s="5" t="s">
         <v>21</v>
       </c>
       <c r="D107">
-        <v>93508.333333333459</v>
-      </c>
-    </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A108" t="s">
+        <v>93508.333333333343</v>
+      </c>
+      <c r="E107">
+        <v>103450</v>
+      </c>
+      <c r="F107" s="4">
+        <v>99707</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A108" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="D108">
-        <v>139.9999999999977</v>
-      </c>
-    </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A109" t="s">
+      <c r="F108" s="4"/>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A109" s="5" t="s">
         <v>22</v>
       </c>
       <c r="D109">
-        <v>28135.000000000044</v>
-      </c>
-    </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A110" t="s">
+        <v>28135</v>
+      </c>
+      <c r="E109">
+        <v>24070</v>
+      </c>
+      <c r="F109" s="4">
+        <v>28574</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A110" s="5" t="s">
         <v>23</v>
       </c>
       <c r="D110">
-        <v>88828.333333333459</v>
-      </c>
-    </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A111" t="s">
+        <v>92786.666666666657</v>
+      </c>
+      <c r="E110">
+        <v>91350</v>
+      </c>
+      <c r="F110" s="4">
+        <v>80767</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A111" s="5" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A112" t="s">
+      <c r="F111" s="4"/>
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A112" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="D112">
-        <v>5844.2708333333412</v>
-      </c>
+      <c r="B112" s="7"/>
+      <c r="C112" s="7"/>
+      <c r="D112" s="7"/>
+      <c r="E112" s="7"/>
+      <c r="F112" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -3016,6 +3510,7 @@
     <mergeCell ref="A94:D94"/>
     <mergeCell ref="A105:D105"/>
   </mergeCells>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
@@ -3025,8 +3520,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7EFBA70C-A8ED-4C94-8FF2-9C7F6AB93B1B}">
   <dimension ref="A1:G145"/>
   <sheetViews>
-    <sheetView topLeftCell="A91" workbookViewId="0">
-      <selection activeCell="D122" sqref="D122"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H108" sqref="H108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3039,13 +3534,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
@@ -4154,13 +4649,13 @@
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A72" s="19" t="s">
+      <c r="A72" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="B72" s="19"/>
-      <c r="C72" s="19"/>
-      <c r="D72" s="19"/>
-      <c r="E72" s="19"/>
+      <c r="B72" s="20"/>
+      <c r="C72" s="20"/>
+      <c r="D72" s="20"/>
+      <c r="E72" s="20"/>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
@@ -4472,13 +4967,13 @@
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A94" s="19" t="s">
+      <c r="A94" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="B94" s="19"/>
-      <c r="C94" s="19"/>
-      <c r="D94" s="19"/>
-      <c r="E94" s="19"/>
+      <c r="B94" s="20"/>
+      <c r="C94" s="20"/>
+      <c r="D94" s="20"/>
+      <c r="E94" s="20"/>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A95" s="1" t="s">
@@ -4636,13 +5131,13 @@
       </c>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A105" s="19" t="s">
+      <c r="A105" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="B105" s="19"/>
-      <c r="C105" s="19"/>
-      <c r="D105" s="19"/>
-      <c r="E105" s="19"/>
+      <c r="B105" s="20"/>
+      <c r="C105" s="20"/>
+      <c r="D105" s="20"/>
+      <c r="E105" s="20"/>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A106" s="1" t="s">
@@ -4774,11 +5269,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C55DEE44-1884-45EE-808F-D75FB017A4E0}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C55DEE44-1884-45EE-808F-D75FB017A4E0}">
   <dimension ref="A1:F63"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="G40" sqref="G40"/>
+    <sheetView topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4791,12 +5286,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="18"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="22"/>
       <c r="E1" s="11"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -5154,12 +5649,12 @@
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A35" s="16" t="s">
+      <c r="A35" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="B35" s="17"/>
-      <c r="C35" s="17"/>
-      <c r="D35" s="18"/>
+      <c r="B35" s="21"/>
+      <c r="C35" s="21"/>
+      <c r="D35" s="22"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" s="13" t="s">
@@ -5286,14 +5781,14 @@
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A49" s="16" t="s">
+      <c r="A49" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="B49" s="17"/>
-      <c r="C49" s="17"/>
-      <c r="D49" s="17"/>
-      <c r="E49" s="17"/>
-      <c r="F49" s="18"/>
+      <c r="B49" s="21"/>
+      <c r="C49" s="21"/>
+      <c r="D49" s="21"/>
+      <c r="E49" s="21"/>
+      <c r="F49" s="22"/>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
@@ -5391,14 +5886,14 @@
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A59" s="16" t="s">
+      <c r="A59" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="B59" s="17"/>
-      <c r="C59" s="17"/>
-      <c r="D59" s="17"/>
-      <c r="E59" s="17"/>
-      <c r="F59" s="18"/>
+      <c r="B59" s="21"/>
+      <c r="C59" s="21"/>
+      <c r="D59" s="21"/>
+      <c r="E59" s="21"/>
+      <c r="F59" s="22"/>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60" s="2" t="s">
@@ -5443,7 +5938,6 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -5464,13 +5958,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
@@ -6576,13 +7070,13 @@
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A72" s="19" t="s">
+      <c r="A72" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="B72" s="20"/>
-      <c r="C72" s="20"/>
-      <c r="D72" s="20"/>
-      <c r="E72" s="20"/>
+      <c r="B72" s="23"/>
+      <c r="C72" s="23"/>
+      <c r="D72" s="23"/>
+      <c r="E72" s="23"/>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
@@ -6894,13 +7388,13 @@
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A94" s="19" t="s">
+      <c r="A94" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="B94" s="20"/>
-      <c r="C94" s="20"/>
-      <c r="D94" s="20"/>
-      <c r="E94" s="20"/>
+      <c r="B94" s="23"/>
+      <c r="C94" s="23"/>
+      <c r="D94" s="23"/>
+      <c r="E94" s="23"/>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A95" s="1" t="s">
@@ -7185,13 +7679,13 @@
       </c>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A113" s="19" t="s">
+      <c r="A113" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="B113" s="20"/>
-      <c r="C113" s="20"/>
-      <c r="D113" s="20"/>
-      <c r="E113" s="20"/>
+      <c r="B113" s="23"/>
+      <c r="C113" s="23"/>
+      <c r="D113" s="23"/>
+      <c r="E113" s="23"/>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A114" s="1" t="s">
@@ -7321,13 +7815,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
@@ -8436,13 +8930,13 @@
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A72" s="19" t="s">
+      <c r="A72" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="B72" s="19"/>
-      <c r="C72" s="19"/>
-      <c r="D72" s="19"/>
-      <c r="E72" s="19"/>
+      <c r="B72" s="20"/>
+      <c r="C72" s="20"/>
+      <c r="D72" s="20"/>
+      <c r="E72" s="20"/>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
@@ -8754,13 +9248,13 @@
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A94" s="19" t="s">
+      <c r="A94" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="B94" s="19"/>
-      <c r="C94" s="19"/>
-      <c r="D94" s="19"/>
-      <c r="E94" s="19"/>
+      <c r="B94" s="20"/>
+      <c r="C94" s="20"/>
+      <c r="D94" s="20"/>
+      <c r="E94" s="20"/>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A95" s="1" t="s">
@@ -9047,13 +9541,13 @@
       <c r="G112" s="9"/>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A113" s="19" t="s">
+      <c r="A113" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="B113" s="20"/>
-      <c r="C113" s="20"/>
-      <c r="D113" s="20"/>
-      <c r="E113" s="20"/>
+      <c r="B113" s="23"/>
+      <c r="C113" s="23"/>
+      <c r="D113" s="23"/>
+      <c r="E113" s="23"/>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A114" s="1" t="s">

</xml_diff>